<commit_message>
Enums for Module, Intent, Language, LanguageCode. Complete Implementation of Introduction Module (Module 1) Session variables for storing persisting parameters. Firestore Database Setup for Custom Responses.
</commit_message>
<xml_diff>
--- a/intent-definition.xlsx
+++ b/intent-definition.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\User\Documents\Code\Thesis\Symptom-Checker-Chatbot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA7D31D1-2CC3-404D-B977-41486B3A33CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ADCB797-7CF1-42E9-B306-467CD13DA83C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="base" sheetId="11" r:id="rId1"/>
-    <sheet name="intents" sheetId="13" r:id="rId2"/>
+    <sheet name="intents-en" sheetId="13" r:id="rId2"/>
+    <sheet name="intents-tl" sheetId="15" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="89">
   <si>
     <t>parameters</t>
   </si>
@@ -170,33 +171,12 @@
     <t>Fulfillment</t>
   </si>
   <si>
-    <t>Hello,Hi,Hey,What's up,Good morning</t>
-  </si>
-  <si>
-    <t>Check up,Evaluate me,Examine me</t>
-  </si>
-  <si>
     <t>What is your preferred language? (English / Tagalog)., Do you wish to speak in Tagalog or English?</t>
   </si>
   <si>
     <t>Do you agree to these terms?</t>
   </si>
   <si>
-    <t>COMMD.CHECK</t>
-  </si>
-  <si>
-    <t>COMMD.GREET</t>
-  </si>
-  <si>
-    <t>ANSWR.LANG</t>
-  </si>
-  <si>
-    <t>ANSWR.YES</t>
-  </si>
-  <si>
-    <t>ANSWR.NO</t>
-  </si>
-  <si>
     <t>QUEST.LANG</t>
   </si>
   <si>
@@ -219,6 +199,96 @@
   </si>
   <si>
     <t>QUEST.PHYSICAL.DRESS</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>action</t>
+  </si>
+  <si>
+    <t>test.slot.filling</t>
+  </si>
+  <si>
+    <t>greeting</t>
+  </si>
+  <si>
+    <t>checkup</t>
+  </si>
+  <si>
+    <t>Hi,Magandang  umaga,Kamusta,Magandang gabi,Hello</t>
+  </si>
+  <si>
+    <t>Hello|Hi|Hey|What's up|Good morning</t>
+  </si>
+  <si>
+    <t>Check up|Evaluate me|Examine me|Test me|Help me</t>
+  </si>
+  <si>
+    <t>Yes|Okay I will|Why not|Yes that's alright|Yes I do|Exactly|Of course|Yep that's ok|Okay|Ok</t>
+  </si>
+  <si>
+    <t>GREETING</t>
+  </si>
+  <si>
+    <t>CHECKUP</t>
+  </si>
+  <si>
+    <t>PRIVACY-POLICY-YES</t>
+  </si>
+  <si>
+    <t>PRIVACY-POLICY-NO</t>
+  </si>
+  <si>
+    <t>LANGUAGE</t>
+  </si>
+  <si>
+    <t>LANGUAGE-SET</t>
+  </si>
+  <si>
+    <t>LANGUAGE-CHANGE</t>
+  </si>
+  <si>
+    <t>No way|No|Na|I can't|No I cannot|Don't|Nope|I disagree|Of course not|No thanks|Not right now|Nah</t>
+  </si>
+  <si>
+    <t>{@language:language:1:0}</t>
+  </si>
+  <si>
+    <t>{@language:english}|I want {@language:tagalog}|I choose {@language:filipino}|{@language:english} please|Let's go with {@language:tagalog}|Change it to {@language:filipino}|Use {@language:filipino} instead</t>
+  </si>
+  <si>
+    <t>I want to change my language|Let me change language|Change language|Change my language to {@language:english}|Use {@language:english} instead</t>
+  </si>
+  <si>
+    <t>{@language:language:0:0}</t>
+  </si>
+  <si>
+    <t>PRIVACY_POLICY</t>
+  </si>
+  <si>
+    <t>I'm sorry, please answer the question. Do you agree to my terms of service?|Sorry? Do you agree to my terms of service?</t>
+  </si>
+  <si>
+    <t>What language?|Sorry, I did not quite get that. What language do you prefer?</t>
+  </si>
+  <si>
+    <t>language_set</t>
+  </si>
+  <si>
+    <t>privacy_policy_yes</t>
+  </si>
+  <si>
+    <t>privacy_policy_no</t>
+  </si>
+  <si>
+    <t>language_change</t>
+  </si>
+  <si>
+    <t>fallback_privacy_policy</t>
+  </si>
+  <si>
+    <t>fallback_language_set</t>
   </si>
 </sst>
 </file>
@@ -1105,10 +1175,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08CBFBF2-BC64-48B4-A624-4A1B2A006627}">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1122,7 +1192,7 @@
     <col min="12" max="16384" width="16.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -1159,8 +1229,11 @@
       <c r="L1" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M1" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -1188,8 +1261,11 @@
       <c r="I2" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M2" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -1206,7 +1282,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>32</v>
       </c>
@@ -1232,7 +1308,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" ht="45" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>33</v>
       </c>
@@ -1264,7 +1340,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>34</v>
       </c>
@@ -1290,7 +1366,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>40</v>
       </c>
@@ -1325,7 +1401,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>46</v>
       </c>
@@ -1345,8 +1421,66 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="4">
+        <v>2</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0</v>
+      </c>
       <c r="J10" s="3"/>
+    </row>
+    <row r="15" spans="1:13" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>58</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1356,10 +1490,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{563BB99E-AECF-4E9F-90DC-16BA1EB2C1A9}">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1373,7 +1507,7 @@
     <col min="12" max="16384" width="16.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -1410,112 +1544,305 @@
       <c r="L1" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="M1" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" s="4">
         <v>0</v>
       </c>
+      <c r="G2" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="H2" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="4">
         <v>0</v>
       </c>
+      <c r="G3" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="H3" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="45" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="78.75" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="4">
+        <v>2</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="56.25" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="4">
+        <v>1</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="L7" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="33.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" ht="45" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>58</v>
+        <v>88</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0</v>
+      </c>
+      <c r="D9" s="4">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>72</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>52</v>
-      </c>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="J10" s="3"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
     </row>
-    <row r="18" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AF69D1E-B293-4AC9-BAA2-CC12BCEF0879}">
+  <dimension ref="A1:M16"/>
+  <sheetViews>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13" style="4" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" style="4" customWidth="1"/>
+    <col min="5" max="7" width="12.7109375" style="1" customWidth="1"/>
+    <col min="8" max="11" width="25.7109375" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="16.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>65</v>
-      </c>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L7" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="J10" s="3"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
General Questions Module Webhooks
</commit_message>
<xml_diff>
--- a/intent-definition.xlsx
+++ b/intent-definition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\User\Documents\Code\Thesis\Symptom-Checker-Chatbot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ADCB797-7CF1-42E9-B306-467CD13DA83C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C8A3648-BE03-42C2-A72A-4C7604B641D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="105">
   <si>
     <t>parameters</t>
   </si>
@@ -289,6 +289,54 @@
   </si>
   <si>
     <t>fallback_language_set</t>
+  </si>
+  <si>
+    <t>name_set</t>
+  </si>
+  <si>
+    <t>sex_set</t>
+  </si>
+  <si>
+    <t>age_set</t>
+  </si>
+  <si>
+    <t>GENERAL</t>
+  </si>
+  <si>
+    <t>{@sys.any:name:1:0}</t>
+  </si>
+  <si>
+    <t>AGE</t>
+  </si>
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>SEX</t>
+  </si>
+  <si>
+    <t>{@sex:sex:1:0}</t>
+  </si>
+  <si>
+    <t>{@sys.age:age:1:0}</t>
+  </si>
+  <si>
+    <t>fallback_age_set</t>
+  </si>
+  <si>
+    <t>fallback_name_set</t>
+  </si>
+  <si>
+    <t>fallback_sex_set</t>
+  </si>
+  <si>
+    <t>general</t>
+  </si>
+  <si>
+    <t>initial_symptom_set</t>
+  </si>
+  <si>
+    <t>INITIAL</t>
   </si>
 </sst>
 </file>
@@ -1490,10 +1538,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{563BB99E-AECF-4E9F-90DC-16BA1EB2C1A9}">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1727,12 +1775,169 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="J10" s="3"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
+      <c r="A10" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="4">
+        <v>1</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="4">
+        <v>2</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="4">
+        <v>2</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="4">
+        <v>2</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="4">
+        <v>1</v>
+      </c>
+      <c r="D14" s="4">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="4">
+        <v>0</v>
+      </c>
+      <c r="D19" s="4">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="4">
+        <v>0</v>
+      </c>
+      <c r="D20" s="4">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="4">
+        <v>0</v>
+      </c>
+      <c r="D21" s="4">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>96</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fulfillment for General Questions
</commit_message>
<xml_diff>
--- a/intent-definition.xlsx
+++ b/intent-definition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\User\Documents\Code\Thesis\Symptom-Checker-Chatbot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C8A3648-BE03-42C2-A72A-4C7604B641D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14087BD0-56D9-4B4F-BB81-EFFF2573FD1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="111">
   <si>
     <t>parameters</t>
   </si>
@@ -252,18 +252,12 @@
     <t>No way|No|Na|I can't|No I cannot|Don't|Nope|I disagree|Of course not|No thanks|Not right now|Nah</t>
   </si>
   <si>
-    <t>{@language:language:1:0}</t>
-  </si>
-  <si>
     <t>{@language:english}|I want {@language:tagalog}|I choose {@language:filipino}|{@language:english} please|Let's go with {@language:tagalog}|Change it to {@language:filipino}|Use {@language:filipino} instead</t>
   </si>
   <si>
     <t>I want to change my language|Let me change language|Change language|Change my language to {@language:english}|Use {@language:english} instead</t>
   </si>
   <si>
-    <t>{@language:language:0:0}</t>
-  </si>
-  <si>
     <t>PRIVACY_POLICY</t>
   </si>
   <si>
@@ -303,9 +297,6 @@
     <t>GENERAL</t>
   </si>
   <si>
-    <t>{@sys.any:name:1:0}</t>
-  </si>
-  <si>
     <t>AGE</t>
   </si>
   <si>
@@ -315,12 +306,6 @@
     <t>SEX</t>
   </si>
   <si>
-    <t>{@sex:sex:1:0}</t>
-  </si>
-  <si>
-    <t>{@sys.age:age:1:0}</t>
-  </si>
-  <si>
     <t>fallback_age_set</t>
   </si>
   <si>
@@ -337,6 +322,39 @@
   </si>
   <si>
     <t>INITIAL</t>
+  </si>
+  <si>
+    <t>I am {@sys.age:20 years old}|{@sys.age:30 years old}|I'm {@sys.age:30 years old} right now|{@sys.age:25 old}|{@sys.age:18 years}</t>
+  </si>
+  <si>
+    <t>{@sys.any:Steven}|You can call me {@sys.any:Mark}|Address me as {@sys.any:Robert}|My name is {@sys.any:Maxson}|Call me {@sys.any:Roy}</t>
+  </si>
+  <si>
+    <t>{@sex:male}|I am a {@sex:girl}|I'm a {@sex:man}|My sex is {@sex:female}|My gender is {@sex:male}</t>
+  </si>
+  <si>
+    <t>{@sys.age:$age:1:0}</t>
+  </si>
+  <si>
+    <t>{@sys.any:$name:1:0}</t>
+  </si>
+  <si>
+    <t>{@language:$language:1:0}</t>
+  </si>
+  <si>
+    <t>{@language:$language:0:0}</t>
+  </si>
+  <si>
+    <t>{@sex:$sex:1:0}</t>
+  </si>
+  <si>
+    <t>What name?</t>
+  </si>
+  <si>
+    <t>Again how old are you?|I'm sorry, how old?|I did not get that, what is your age?</t>
+  </si>
+  <si>
+    <t>What sex?|What is your biological sex?</t>
   </si>
 </sst>
 </file>
@@ -1540,8 +1558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{563BB99E-AECF-4E9F-90DC-16BA1EB2C1A9}">
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1638,7 +1656,7 @@
     </row>
     <row r="4" spans="1:13" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>11</v>
@@ -1650,7 +1668,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>70</v>
@@ -1661,7 +1679,7 @@
     </row>
     <row r="5" spans="1:13" ht="45" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>11</v>
@@ -1673,7 +1691,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>71</v>
@@ -1684,7 +1702,7 @@
     </row>
     <row r="6" spans="1:13" ht="78.75" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>11</v>
@@ -1702,15 +1720,15 @@
         <v>73</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>11</v>
@@ -1725,10 +1743,10 @@
         <v>74</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>79</v>
+        <v>106</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>15</v>
@@ -1736,7 +1754,7 @@
     </row>
     <row r="8" spans="1:13" ht="45" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>11</v>
@@ -1748,15 +1766,15 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>11</v>
@@ -1771,12 +1789,12 @@
         <v>72</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>11</v>
@@ -1787,16 +1805,13 @@
       <c r="D10" s="4">
         <v>0</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="G10" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>11</v>
@@ -1808,18 +1823,21 @@
         <v>0</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>100</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>11</v>
@@ -1831,18 +1849,21 @@
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>101</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="45" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>11</v>
@@ -1854,90 +1875,115 @@
         <v>0</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="4">
+        <v>0</v>
+      </c>
+      <c r="D14" s="4">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="4">
+        <v>0</v>
+      </c>
+      <c r="D15" s="4">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="G13" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="4">
+      <c r="B16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0</v>
+      </c>
+      <c r="D16" s="4">
         <v>1</v>
       </c>
-      <c r="D14" s="4">
-        <v>0</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>104</v>
+      <c r="E16" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="4">
+        <v>1</v>
+      </c>
+      <c r="D17" s="4">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="4">
-        <v>0</v>
-      </c>
-      <c r="D19" s="4">
-        <v>1</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>94</v>
-      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" s="4">
-        <v>0</v>
-      </c>
-      <c r="D20" s="4">
-        <v>1</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>95</v>
-      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="4">
-        <v>0</v>
-      </c>
-      <c r="D21" s="4">
-        <v>1</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>96</v>
-      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Initial Setup of Symptom Elicitation Phase Fulfillment. Fixed issues where Messages are not sent in correct order on Messenger.
</commit_message>
<xml_diff>
--- a/intent-definition.xlsx
+++ b/intent-definition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\User\Documents\Code\Thesis\Symptom-Checker-Chatbot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14087BD0-56D9-4B4F-BB81-EFFF2573FD1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EAC546E-6AED-48B0-AA7A-4B2D97F1A06E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="117">
   <si>
     <t>parameters</t>
   </si>
@@ -355,6 +355,24 @@
   </si>
   <si>
     <t>What sex?|What is your biological sex?</t>
+  </si>
+  <si>
+    <t>fallback_symptom_set</t>
+  </si>
+  <si>
+    <t>What symptom?|Could you share one symptom?</t>
+  </si>
+  <si>
+    <t>elicitation</t>
+  </si>
+  <si>
+    <t>ELICITATION</t>
+  </si>
+  <si>
+    <t>{@symptom:cough}|Have a {@symptom:cough}|Got a {@symptom:cough}|Suffering from {@symptom:cough}|Feeling a {@symptom:cough}|This persistent {@symptom:cough}|This {@symptom:cough}|Dealing with {@symptom:cough}|Down with {@symptom:cough}|Struggling with a {@symptom:cough}|Contracted a {@symptom:cough}|Constant {@symptom:cough}</t>
+  </si>
+  <si>
+    <t>{@symptom:$symptom:1:0}</t>
   </si>
 </sst>
 </file>
@@ -874,7 +892,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -885,6 +903,9 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1556,10 +1577,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{563BB99E-AECF-4E9F-90DC-16BA1EB2C1A9}">
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1947,7 +1968,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="135" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>98</v>
       </c>
@@ -1966,24 +1987,54 @@
       <c r="G17" s="1" t="s">
         <v>99</v>
       </c>
+      <c r="H17" s="1" t="s">
+        <v>115</v>
+      </c>
       <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
+      <c r="J17" s="5" t="s">
+        <v>116</v>
+      </c>
       <c r="K17" s="4"/>
     </row>
+    <row r="18" spans="1:11" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="4">
+        <v>0</v>
+      </c>
+      <c r="D18" s="4">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
+      <c r="A19" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="4">
+        <v>1</v>
+      </c>
+      <c r="D19" s="4">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>114</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Initial Setup of Symptom Elicitation Phase Fulfillment.
</commit_message>
<xml_diff>
--- a/intent-definition.xlsx
+++ b/intent-definition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\User\Documents\Code\Thesis\Symptom-Checker-Chatbot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14087BD0-56D9-4B4F-BB81-EFFF2573FD1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EAC546E-6AED-48B0-AA7A-4B2D97F1A06E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="117">
   <si>
     <t>parameters</t>
   </si>
@@ -355,6 +355,24 @@
   </si>
   <si>
     <t>What sex?|What is your biological sex?</t>
+  </si>
+  <si>
+    <t>fallback_symptom_set</t>
+  </si>
+  <si>
+    <t>What symptom?|Could you share one symptom?</t>
+  </si>
+  <si>
+    <t>elicitation</t>
+  </si>
+  <si>
+    <t>ELICITATION</t>
+  </si>
+  <si>
+    <t>{@symptom:cough}|Have a {@symptom:cough}|Got a {@symptom:cough}|Suffering from {@symptom:cough}|Feeling a {@symptom:cough}|This persistent {@symptom:cough}|This {@symptom:cough}|Dealing with {@symptom:cough}|Down with {@symptom:cough}|Struggling with a {@symptom:cough}|Contracted a {@symptom:cough}|Constant {@symptom:cough}</t>
+  </si>
+  <si>
+    <t>{@symptom:$symptom:1:0}</t>
   </si>
 </sst>
 </file>
@@ -874,7 +892,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -885,6 +903,9 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1556,10 +1577,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{563BB99E-AECF-4E9F-90DC-16BA1EB2C1A9}">
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1947,7 +1968,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="135" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>98</v>
       </c>
@@ -1966,24 +1987,54 @@
       <c r="G17" s="1" t="s">
         <v>99</v>
       </c>
+      <c r="H17" s="1" t="s">
+        <v>115</v>
+      </c>
       <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
+      <c r="J17" s="5" t="s">
+        <v>116</v>
+      </c>
       <c r="K17" s="4"/>
     </row>
+    <row r="18" spans="1:11" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="4">
+        <v>0</v>
+      </c>
+      <c r="D18" s="4">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
+      <c r="A19" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="4">
+        <v>1</v>
+      </c>
+      <c r="D19" s="4">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>114</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added Symptom Property Intents
</commit_message>
<xml_diff>
--- a/intent-definition.xlsx
+++ b/intent-definition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\User\Documents\Code\Thesis\Symptom-Checker-Chatbot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EAC546E-6AED-48B0-AA7A-4B2D97F1A06E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{930E92F4-D9EC-42F7-9BBF-A9751C5741CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="248">
   <si>
     <t>parameters</t>
   </si>
@@ -373,6 +373,399 @@
   </si>
   <si>
     <t>{@symptom:$symptom:1:0}</t>
+  </si>
+  <si>
+    <t>HAS</t>
+  </si>
+  <si>
+    <t>has_symptom_yes</t>
+  </si>
+  <si>
+    <t>has_symptom_no</t>
+  </si>
+  <si>
+    <t>HAS-SYMPTOM-YES</t>
+  </si>
+  <si>
+    <t>HAS-SYMPTOM-NO</t>
+  </si>
+  <si>
+    <t>DURATION</t>
+  </si>
+  <si>
+    <t>DURATION-GENERIC</t>
+  </si>
+  <si>
+    <t>DURATION-EXPLICIT</t>
+  </si>
+  <si>
+    <t>{@sys.duration:$duration:1:0}</t>
+  </si>
+  <si>
+    <t>{@duration_generic:$duration:1:0}</t>
+  </si>
+  <si>
+    <t>{@duration_generic:Days}|I had it for {@duration_generic:weeks}|A couple {@duration_generic:days}|About a {@duration_generic:Day}|Around a {@duration_generic:Month}</t>
+  </si>
+  <si>
+    <t>fallback_has_symptom</t>
+  </si>
+  <si>
+    <t>fallback_duration</t>
+  </si>
+  <si>
+    <t>Again how long?</t>
+  </si>
+  <si>
+    <t>Again do you have it?</t>
+  </si>
+  <si>
+    <t>{@sys.duration:2 days}|It has been {@sys.duration:3 days}|About {@sys.duration:4 days}|Around {@sys.duration:5 days}|I had it for {@sys.duration:5 days}|{@sys.duration:5 days} has passed|A {@sys.duration:1 Month}</t>
+  </si>
+  <si>
+    <t>duration_generic_set</t>
+  </si>
+  <si>
+    <t>duration_explicit_set</t>
+  </si>
+  <si>
+    <t>Yes|Okay I will|Why not|Yes that's alright|Yes I do|Exactly|Of course|Yep that's ok|Okay|Ok|I have it</t>
+  </si>
+  <si>
+    <t>No way|No|Na|I can't|No I cannot|Don't|Nope|I disagree|Of course not|No thanks|Not right now|Nah|I don't|Don't have it</t>
+  </si>
+  <si>
+    <t>developer_context</t>
+  </si>
+  <si>
+    <t>developer_jump</t>
+  </si>
+  <si>
+    <t>CTX {@sys.any:$any:1:0}</t>
+  </si>
+  <si>
+    <t>JMP {@sys.any:$any:1:0}</t>
+  </si>
+  <si>
+    <t>{@sys.any:$any:1:0}</t>
+  </si>
+  <si>
+    <t>weight_set</t>
+  </si>
+  <si>
+    <t>WEIGHT</t>
+  </si>
+  <si>
+    <t>fallback_weight</t>
+  </si>
+  <si>
+    <t>temperature_body</t>
+  </si>
+  <si>
+    <t>fallback_temperature_body</t>
+  </si>
+  <si>
+    <t>TEMPERATURE</t>
+  </si>
+  <si>
+    <t>Again how heavy?</t>
+  </si>
+  <si>
+    <t>TEMPERATURE-BODY</t>
+  </si>
+  <si>
+    <t>Again what is your temperature?</t>
+  </si>
+  <si>
+    <t>{@sys.unit-weight: 60kg}|I am {@sys.unit-weight: 60kg}|I weigh {@sys.unit-weight: 60kg}|Around {@sys.unit-weight: 60kg}|About {@sys.unit-weight: 60kg}</t>
+  </si>
+  <si>
+    <t>{@sys.unit-weight:$weight:1:0}</t>
+  </si>
+  <si>
+    <t>{@sys.temperature: 38°}|My body is {@sys.temperature: 38 C}|Around {@sys.temperature: 38°}|About {@sys.temperature: 38C}|It is {@sys.temperature: 38 degrees}</t>
+  </si>
+  <si>
+    <t>{@sys.temperature:$temperature:1:0}</t>
+  </si>
+  <si>
+    <t>frequency_adverbs_set</t>
+  </si>
+  <si>
+    <t>frequency_explicit_set</t>
+  </si>
+  <si>
+    <t>fallback_frequency</t>
+  </si>
+  <si>
+    <t>FREQUENCY</t>
+  </si>
+  <si>
+    <t>FREQUENCY-ADVERBS</t>
+  </si>
+  <si>
+    <t>FREQUENCY-EXPLICIT</t>
+  </si>
+  <si>
+    <t>Again how often?</t>
+  </si>
+  <si>
+    <t>{@frequency_adverbs:$frequency:1:0}</t>
+  </si>
+  <si>
+    <t>{@sys.duration:$frequency:1:0}</t>
+  </si>
+  <si>
+    <t>{@frequency_adverbs:sometimes}|{@frequency_adverbs:often} when|It happens {@frequency_adverbs:weekly}|I have it {@frequency_adverbs:daily}|Very {@frequency_adverbs:frequent}|{@frequency_adverbs:sometimes} a lot|It occurs {@frequency_adverbs:sometimes}|It get it {@frequency_adverbs:sometimes}</t>
+  </si>
+  <si>
+    <t>{@sys.duration:2 days}|I have it for {@sys.duration:2 weeks} now|About {@sys.duration:2 weeks}|Around {@sys.duration:3 weeks}|Got it for {@sys.duration:2 weeks}|It has happened for {@sys.duration:2 weeks}|{@sys.duration:2 weeks} long|Every {@sys.duration:2 weeks}</t>
+  </si>
+  <si>
+    <t>pain_intensity_set</t>
+  </si>
+  <si>
+    <t>weakness_intensity_set</t>
+  </si>
+  <si>
+    <t>PAIN-INTENSITY</t>
+  </si>
+  <si>
+    <t>WEAKNESS-INTENSITY</t>
+  </si>
+  <si>
+    <t>{@intensity:1}|Around {@intensity:2}|I give it a {@intensity:3}|A scale of {@intensity:4}|An intensity of {@intensity:5}|I think its a {@intensity:6}|{@intensity:7} strong|{@intensity:8} weak|Level {@intensity:9}|Approximately {@intensity:10}</t>
+  </si>
+  <si>
+    <t>PAIN</t>
+  </si>
+  <si>
+    <t>WEAKNESS</t>
+  </si>
+  <si>
+    <t>fallback_pain</t>
+  </si>
+  <si>
+    <t>fallback_weakness</t>
+  </si>
+  <si>
+    <t>Again how painful?</t>
+  </si>
+  <si>
+    <t>Again how weak?</t>
+  </si>
+  <si>
+    <t>{@intensity:$intensity:1:0}</t>
+  </si>
+  <si>
+    <t>pain_adjectives_set</t>
+  </si>
+  <si>
+    <t>PAIN-ADJECTIVES</t>
+  </si>
+  <si>
+    <t>{@pain_adjectives:severe}|I feel a {@pain_adjectives:slight} pain|It is {@pain_adjectives:dull}|A {@pain_adjectives:severe} pain|It feels {@pain_adjectives:severe}</t>
+  </si>
+  <si>
+    <t>{@pain_adjectives:$adjectives:1:0}</t>
+  </si>
+  <si>
+    <t>location_eyes_set</t>
+  </si>
+  <si>
+    <t>location_body_locale_set</t>
+  </si>
+  <si>
+    <t>location_body_region_set</t>
+  </si>
+  <si>
+    <t>fallback_location_eyes</t>
+  </si>
+  <si>
+    <t>fallback_location_locale</t>
+  </si>
+  <si>
+    <t>fallback_location_region</t>
+  </si>
+  <si>
+    <t>LOCALE</t>
+  </si>
+  <si>
+    <t>EYES</t>
+  </si>
+  <si>
+    <t>REGION</t>
+  </si>
+  <si>
+    <t>LOCATION-EYES</t>
+  </si>
+  <si>
+    <t>LOCATION-LOCALE</t>
+  </si>
+  <si>
+    <t>LOCATION-REGION</t>
+  </si>
+  <si>
+    <t>{@location_eyes:$eyes:1:0}</t>
+  </si>
+  <si>
+    <t>{@location_body_locale:$locale:1:0}</t>
+  </si>
+  <si>
+    <t>{@location_body_region:$region:1:0}</t>
+  </si>
+  <si>
+    <t>Again which eye?</t>
+  </si>
+  <si>
+    <t>Again what body part?</t>
+  </si>
+  <si>
+    <t>Again is it general or localized?</t>
+  </si>
+  <si>
+    <t>{@location_eyes:left}|The {@location_eyes:left} eye|It on the {@location_eyes:left}|{@location_eyes:left} eyes|My {@location_eyes:left} eye|I feel it on my {@location_eyes:left} eye</t>
+  </si>
+  <si>
+    <t>{@location_body_locale:head}|My {@location_body_locale:head}|I feel it on my {@location_body_locale:head}|On my {@location_body_locale:head}|It hurts on my {@location_body_locale:head}|Around my {@location_body_locale:head} area|{@location_body_locale:head} area</t>
+  </si>
+  <si>
+    <t>{@location_body_region:localized}|It is {@location_body_region:localized}|In {@location_body_region:localized} region</t>
+  </si>
+  <si>
+    <t>color_phlegm_set</t>
+  </si>
+  <si>
+    <t>COLOR</t>
+  </si>
+  <si>
+    <t>fallback_color</t>
+  </si>
+  <si>
+    <t>COLOR-PHLEGM</t>
+  </si>
+  <si>
+    <t>Again what color?</t>
+  </si>
+  <si>
+    <t>{@color_phlegm:green}|It is color {@color_phlegm:green}|Color {@color_phlegm:green}|It is {@color_phlegm:green}|It looks {@color_phlegm:green}|has a {@color_phlegm:green} hue</t>
+  </si>
+  <si>
+    <t>difficulty_set</t>
+  </si>
+  <si>
+    <t>fallback_difficulty</t>
+  </si>
+  <si>
+    <t>DIFFICULTY</t>
+  </si>
+  <si>
+    <t>Again how hard?</t>
+  </si>
+  <si>
+    <t>moisture_set</t>
+  </si>
+  <si>
+    <t>fallback_moisture</t>
+  </si>
+  <si>
+    <t>MOISTURE</t>
+  </si>
+  <si>
+    <t>Again is it dry or wet?</t>
+  </si>
+  <si>
+    <t>physical_state_set</t>
+  </si>
+  <si>
+    <t>fallback_physical</t>
+  </si>
+  <si>
+    <t>PHYSICAL</t>
+  </si>
+  <si>
+    <t>Againt is it at rest or during activity?</t>
+  </si>
+  <si>
+    <t>{@color_phlegm:$color:1:0}</t>
+  </si>
+  <si>
+    <t>{@difficulty:$difficulty:1:0}</t>
+  </si>
+  <si>
+    <t>{@moisture:$moisture:1:0}</t>
+  </si>
+  <si>
+    <t>{@physical_state:$physical:1:0}</t>
+  </si>
+  <si>
+    <t>{@difficulty:easy}|It is {@difficulty:easy}|I find it {@difficulty:easy}|Very {@difficulty:easy}|Just {@difficulty: hard}</t>
+  </si>
+  <si>
+    <t>{@moisture:wet}|It is {@moisture:wet}|Very {@moisture:wet}|I feels {@moisture:wet}|Just {@moisture:wet}</t>
+  </si>
+  <si>
+    <t>{@physical_state:rest}|During {@physical_state:rest}|At {@physical_state:rest}|It happens during {@physical_state:rest}|While {@physical_state:rest}</t>
+  </si>
+  <si>
+    <t>count_set</t>
+  </si>
+  <si>
+    <t>inteference_yes</t>
+  </si>
+  <si>
+    <t>inteference_no</t>
+  </si>
+  <si>
+    <t>parts_day_set</t>
+  </si>
+  <si>
+    <t>COUNT</t>
+  </si>
+  <si>
+    <t>PARTS</t>
+  </si>
+  <si>
+    <t>INTERFERENCE</t>
+  </si>
+  <si>
+    <t>fallback_count</t>
+  </si>
+  <si>
+    <t>fallback_inteference</t>
+  </si>
+  <si>
+    <t>fallback_parts</t>
+  </si>
+  <si>
+    <t>INTERFERENCE-YES</t>
+  </si>
+  <si>
+    <t>INTERFERENCE-NO</t>
+  </si>
+  <si>
+    <t>PARTS-DAY</t>
+  </si>
+  <si>
+    <t>Again how many times?</t>
+  </si>
+  <si>
+    <t>Did it intefere?</t>
+  </si>
+  <si>
+    <t>What time of the day?</t>
+  </si>
+  <si>
+    <t>{@parts_day:$parts:1:0}</t>
+  </si>
+  <si>
+    <t>{@sys.number:$number:1:0}</t>
+  </si>
+  <si>
+    <t>{@sys.number:2}|{@sys.number:2} times|Around {@sys.number:2} times|Over {@sys.number:2} times|{@sys.number:2} already</t>
+  </si>
+  <si>
+    <t>{@parts_day:morning}|In the {@parts_day:morning}|At {@parts_day:morning}|during {@parts_day:morning}|around the {@parts_day:morning}</t>
   </si>
 </sst>
 </file>
@@ -952,7 +1345,15 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1577,19 +1978,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{563BB99E-AECF-4E9F-90DC-16BA1EB2C1A9}">
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:M60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="13" style="4" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" style="4" customWidth="1"/>
     <col min="4" max="4" width="9.5703125" style="4" customWidth="1"/>
-    <col min="5" max="7" width="12.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" style="1" customWidth="1"/>
     <col min="8" max="11" width="25.7109375" style="1" customWidth="1"/>
     <col min="12" max="16384" width="16.140625" style="1"/>
   </cols>
@@ -2034,6 +2437,949 @@
       </c>
       <c r="G19" s="1" t="s">
         <v>114</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="4">
+        <v>1</v>
+      </c>
+      <c r="D20" s="4">
+        <v>0</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="4">
+        <v>1</v>
+      </c>
+      <c r="D21" s="4">
+        <v>0</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="45" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="4">
+        <v>1</v>
+      </c>
+      <c r="D22" s="4">
+        <v>0</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="45" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="4">
+        <v>1</v>
+      </c>
+      <c r="D23" s="4">
+        <v>0</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="4">
+        <v>0</v>
+      </c>
+      <c r="D24" s="4">
+        <v>1</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="67.5" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="4">
+        <v>1</v>
+      </c>
+      <c r="D25" s="4">
+        <v>0</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="78.75" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="4">
+        <v>1</v>
+      </c>
+      <c r="D26" s="4">
+        <v>0</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="4">
+        <v>0</v>
+      </c>
+      <c r="D27" s="4">
+        <v>1</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="56.25" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="4">
+        <v>1</v>
+      </c>
+      <c r="D28" s="4">
+        <v>0</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="4">
+        <v>0</v>
+      </c>
+      <c r="D29" s="4">
+        <v>1</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="56.25" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="4">
+        <v>1</v>
+      </c>
+      <c r="D30" s="4">
+        <v>0</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" s="4">
+        <v>0</v>
+      </c>
+      <c r="D31" s="4">
+        <v>1</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="135" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" s="4">
+        <v>1</v>
+      </c>
+      <c r="D32" s="4">
+        <v>0</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="101.25" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="4">
+        <v>1</v>
+      </c>
+      <c r="D33" s="4">
+        <v>0</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" s="4">
+        <v>0</v>
+      </c>
+      <c r="D34" s="4">
+        <v>1</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="101.25" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" s="4">
+        <v>1</v>
+      </c>
+      <c r="D35" s="4">
+        <v>0</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="101.25" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" s="4">
+        <v>1</v>
+      </c>
+      <c r="D36" s="4">
+        <v>0</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" s="4">
+        <v>0</v>
+      </c>
+      <c r="D37" s="4">
+        <v>1</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" s="4">
+        <v>0</v>
+      </c>
+      <c r="D38" s="4">
+        <v>1</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="56.25" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39" s="4">
+        <v>1</v>
+      </c>
+      <c r="D39" s="4">
+        <v>0</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="67.5" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" s="4">
+        <v>1</v>
+      </c>
+      <c r="D40" s="4">
+        <v>0</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="135" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" s="4">
+        <v>1</v>
+      </c>
+      <c r="D41" s="4">
+        <v>0</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="67.5" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42" s="4">
+        <v>1</v>
+      </c>
+      <c r="D42" s="4">
+        <v>0</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C43" s="4">
+        <v>0</v>
+      </c>
+      <c r="D43" s="4">
+        <v>1</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44" s="4">
+        <v>0</v>
+      </c>
+      <c r="D44" s="4">
+        <v>1</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C45" s="4">
+        <v>0</v>
+      </c>
+      <c r="D45" s="4">
+        <v>1</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="67.5" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C46" s="4">
+        <v>1</v>
+      </c>
+      <c r="D46" s="4">
+        <v>0</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C47" s="4">
+        <v>0</v>
+      </c>
+      <c r="D47" s="4">
+        <v>1</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="56.25" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C48" s="4">
+        <v>1</v>
+      </c>
+      <c r="D48" s="4">
+        <v>0</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C49" s="4">
+        <v>0</v>
+      </c>
+      <c r="D49" s="4">
+        <v>1</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="56.25" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C50" s="4">
+        <v>1</v>
+      </c>
+      <c r="D50" s="4">
+        <v>0</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C51" s="4">
+        <v>0</v>
+      </c>
+      <c r="D51" s="4">
+        <v>1</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="67.5" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C52" s="4">
+        <v>1</v>
+      </c>
+      <c r="D52" s="4">
+        <v>0</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="J52" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C53" s="4">
+        <v>0</v>
+      </c>
+      <c r="D53" s="4">
+        <v>1</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C54" s="4">
+        <v>1</v>
+      </c>
+      <c r="D54" s="4">
+        <v>0</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="J54" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C55" s="4">
+        <v>1</v>
+      </c>
+      <c r="D55" s="4">
+        <v>0</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C56" s="4">
+        <v>1</v>
+      </c>
+      <c r="D56" s="4">
+        <v>0</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="56.25" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C57" s="4">
+        <v>1</v>
+      </c>
+      <c r="D57" s="4">
+        <v>0</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C58" s="4">
+        <v>0</v>
+      </c>
+      <c r="D58" s="4">
+        <v>1</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C59" s="4">
+        <v>0</v>
+      </c>
+      <c r="D59" s="4">
+        <v>1</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C60" s="4">
+        <v>0</v>
+      </c>
+      <c r="D60" s="4">
+        <v>1</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>243</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Complete Symptom Property Intents
</commit_message>
<xml_diff>
--- a/intent-definition.xlsx
+++ b/intent-definition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\User\Documents\Code\Thesis\Symptom-Checker-Chatbot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{930E92F4-D9EC-42F7-9BBF-A9751C5741CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{188B5497-9CC8-4783-8BEC-D2F7B0054AD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="293">
   <si>
     <t>parameters</t>
   </si>
@@ -324,9 +324,6 @@
     <t>INITIAL</t>
   </si>
   <si>
-    <t>I am {@sys.age:20 years old}|{@sys.age:30 years old}|I'm {@sys.age:30 years old} right now|{@sys.age:25 old}|{@sys.age:18 years}</t>
-  </si>
-  <si>
     <t>{@sys.any:Steven}|You can call me {@sys.any:Mark}|Address me as {@sys.any:Robert}|My name is {@sys.any:Maxson}|Call me {@sys.any:Roy}</t>
   </si>
   <si>
@@ -766,6 +763,144 @@
   </si>
   <si>
     <t>{@parts_day:morning}|In the {@parts_day:morning}|At {@parts_day:morning}|during {@parts_day:morning}|around the {@parts_day:morning}</t>
+  </si>
+  <si>
+    <t>HEARTRATE</t>
+  </si>
+  <si>
+    <t>heartrate_set</t>
+  </si>
+  <si>
+    <t>fallback_heartrate</t>
+  </si>
+  <si>
+    <t>{@heartrate:$heartrate:1:0}</t>
+  </si>
+  <si>
+    <t>blood_pressure_set</t>
+  </si>
+  <si>
+    <t>PRESSURE</t>
+  </si>
+  <si>
+    <t>fallback_pressure</t>
+  </si>
+  <si>
+    <t>Again what is your blood pressure? x/y</t>
+  </si>
+  <si>
+    <t>{@blood_pressure:$blood_pressure:1:0}</t>
+  </si>
+  <si>
+    <t>{@heartrate:120}|{@heartrate:90} bpm|{@heartrate:40} beats|{@heartrate:79} beats per minute|My heartrate is {@heartrate:88}|Heartrate of {@heartrate:111}|Rate of {@heartrate:120}|It is {@heartrate:80}</t>
+  </si>
+  <si>
+    <t>{@blood_pressure:120/90}|My blood pressure is {@blood_pressure:30/90}|It is {@blood_pressure:110/80}|My BP is {@blood_pressure:25/44}|It measures {@blood_pressure:77/91}|Around {@blood_pressure:112/94}|About {@blood_pressure:140/93}|It levels {@blood_pressure:130/78}</t>
+  </si>
+  <si>
+    <t>Again what is your heartrate? (x bpm)</t>
+  </si>
+  <si>
+    <t>I am {@sys.age:20 years old}|{@sys.age:30 years old}|I'm {@sys.age:30 years old} right now|{@sys.age:25} old|{@sys.age:18 years}</t>
+  </si>
+  <si>
+    <t>TRIGGER</t>
+  </si>
+  <si>
+    <t>CHANGE</t>
+  </si>
+  <si>
+    <t>CARDIOVASCULAR</t>
+  </si>
+  <si>
+    <t>RESPIRATORY</t>
+  </si>
+  <si>
+    <t>TRIGGER-ACTIVITY</t>
+  </si>
+  <si>
+    <t>TRIGGER-STATE</t>
+  </si>
+  <si>
+    <t>TRIGGER-FOOD</t>
+  </si>
+  <si>
+    <t>{@trigger_activity:$trigger:1:0}</t>
+  </si>
+  <si>
+    <t>{@trigger_state:$trigger:1:0}</t>
+  </si>
+  <si>
+    <t>{@trigger_food:$trigger:1:0}</t>
+  </si>
+  <si>
+    <t>{@cardiovascular:$cardiovascular:1:0}</t>
+  </si>
+  <si>
+    <t>{@respiratory:$respiratory:1:0}</t>
+  </si>
+  <si>
+    <t>fallback_cardiovascular</t>
+  </si>
+  <si>
+    <t>fallback_trigger</t>
+  </si>
+  <si>
+    <t>fallback_respiratory</t>
+  </si>
+  <si>
+    <t>fallback_change</t>
+  </si>
+  <si>
+    <t>Again what triggered it?</t>
+  </si>
+  <si>
+    <t>Again is there any change?</t>
+  </si>
+  <si>
+    <t>Again any history with cardiovascular disease?</t>
+  </si>
+  <si>
+    <t>Again any history with respiratory disease?</t>
+  </si>
+  <si>
+    <t>{@trigger_activity:walking}|during {@trigger_activity:walking}|while {@trigger_activity:walking}|happened when {@trigger_activity:walking}|trigger by {@trigger_activity:walking}|by {@trigger_activity:walking}|cause by {@trigger_activity:walking}|I was {@trigger_activity:walking}</t>
+  </si>
+  <si>
+    <t>{@trigger_state:stressed}|When {@trigger_state:stressed}|I was {@trigger_state:stressed}|during {@trigger_state:stressed}|I had {@trigger_state:stressed}|felt {@trigger_state:stressed}|was {@trigger_state:stressed}|{@trigger_state:stressed} triggered it|happened when I {@trigger_state:stressed}</t>
+  </si>
+  <si>
+    <t>{@trigger_food:milk}|eating {@trigger_food:milk}|drinking {@trigger_food:milk}|consuming {@trigger_food:milk}|when I had {@trigger_food:milk}|had {@trigger_food:milk}|took {@trigger_food:milk}|tried {@trigger_food:milk}</t>
+  </si>
+  <si>
+    <t>{@cardiovascular:heart failure}|I had {@cardiovascular:heart failure}|My family had {@cardiovascular:heart failure}|have history in {@cardiovascular:heart failure}|My mom side has {@cardiovascular:heart failure}|My dad side has {@cardiovascular:heart failure}|We have history with {@cardiovascular:heart failure}|I got {@cardiovascular:heart failure}|had {@cardiovascular:heart failure}</t>
+  </si>
+  <si>
+    <t>{@respiratory:asthma}|I had {@respiratory:asthma}|My family had {@respiratory:asthma}|have history in {@respiratory:asthma}|My mom side has {@respiratory:asthma}|My dad side has {@respiratory:asthma}|We have history with {@respiratory:asthma}|I got {@respiratory:asthma}|had {@respiratory:asthma}</t>
+  </si>
+  <si>
+    <t>{@change_quantity:increase}|it {@change_quantity:increase}|has {@change_quantity:increase}|there is an {@change_quantity:increase}|I notice {@change_quantity:increase}|gradually {@change_quantity:increase}|was {@change_quantity:increase}|it is {@change_quantity:increase}</t>
+  </si>
+  <si>
+    <t>{@change_quantity:$change:1:0}</t>
+  </si>
+  <si>
+    <t>trigger_activity_set</t>
+  </si>
+  <si>
+    <t>trigger_state_set</t>
+  </si>
+  <si>
+    <t>trigger_food_set</t>
+  </si>
+  <si>
+    <t>change_quantity_set</t>
+  </si>
+  <si>
+    <t>cardiovascular_set</t>
+  </si>
+  <si>
+    <t>respiratory_set</t>
   </si>
 </sst>
 </file>
@@ -1345,15 +1480,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1978,10 +2105,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{563BB99E-AECF-4E9F-90DC-16BA1EB2C1A9}">
-  <dimension ref="A1:M60"/>
+  <dimension ref="A1:M74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G57" sqref="G57"/>
+    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I73" sqref="I73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1993,7 +2120,9 @@
     <col min="5" max="5" width="14.5703125" style="1" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
     <col min="7" max="7" width="14.7109375" style="1" customWidth="1"/>
-    <col min="8" max="11" width="25.7109375" style="1" customWidth="1"/>
+    <col min="8" max="9" width="25.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="26.28515625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="25.7109375" style="1" customWidth="1"/>
     <col min="12" max="16384" width="16.140625" style="1"/>
   </cols>
   <sheetData>
@@ -2147,7 +2276,7 @@
         <v>76</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="56.25" x14ac:dyDescent="0.2">
@@ -2170,7 +2299,7 @@
         <v>77</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>15</v>
@@ -2253,10 +2382,10 @@
         <v>91</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>100</v>
+        <v>259</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="56.25" x14ac:dyDescent="0.2">
@@ -2279,10 +2408,10 @@
         <v>92</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="45" x14ac:dyDescent="0.2">
@@ -2305,10 +2434,10 @@
         <v>93</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="33.75" x14ac:dyDescent="0.2">
@@ -2328,7 +2457,7 @@
         <v>91</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
@@ -2348,7 +2477,7 @@
         <v>92</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="22.5" x14ac:dyDescent="0.2">
@@ -2368,7 +2497,7 @@
         <v>93</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="135" x14ac:dyDescent="0.2">
@@ -2391,17 +2520,17 @@
         <v>99</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I17" s="4"/>
       <c r="J17" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K17" s="4"/>
     </row>
     <row r="18" spans="1:11" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>11</v>
@@ -2416,32 +2545,32 @@
         <v>99</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="4">
+        <v>1</v>
+      </c>
+      <c r="D19" s="4">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="4">
-        <v>1</v>
-      </c>
-      <c r="D19" s="4">
-        <v>0</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>114</v>
-      </c>
       <c r="G19" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>11</v>
@@ -2453,15 +2582,15 @@
         <v>0</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>11</v>
@@ -2473,61 +2602,55 @@
         <v>0</v>
       </c>
       <c r="H21" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="J21" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="J21" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C22" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D22" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="45" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C23" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="G23" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="H23" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="I23" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>128</v>
+        <v>143</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>11</v>
@@ -2539,67 +2662,55 @@
         <v>1</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>117</v>
+        <v>142</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="67.5" x14ac:dyDescent="0.2">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C25" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D25" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="78.75" x14ac:dyDescent="0.2">
+        <v>146</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>134</v>
+        <v>156</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C26" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D26" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>125</v>
+        <v>157</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>129</v>
+        <v>172</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>11</v>
@@ -2611,41 +2722,35 @@
         <v>1</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>122</v>
+        <v>170</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="56.25" x14ac:dyDescent="0.2">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>142</v>
+        <v>173</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C28" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D28" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>152</v>
+        <v>171</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>144</v>
+        <v>184</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>11</v>
@@ -2657,41 +2762,35 @@
         <v>1</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>143</v>
+        <v>188</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="56.25" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>145</v>
+        <v>185</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C30" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D30" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="J30" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="22.5" x14ac:dyDescent="0.2">
+        <v>187</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>146</v>
+        <v>186</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>11</v>
@@ -2703,67 +2802,55 @@
         <v>1</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>147</v>
+        <v>189</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" ht="135" x14ac:dyDescent="0.2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>155</v>
+        <v>204</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C32" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D32" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="J32" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="101.25" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>156</v>
+        <v>209</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C33" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D33" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="J33" s="1" t="s">
-        <v>163</v>
+        <v>210</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>157</v>
+        <v>213</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>11</v>
@@ -2775,67 +2862,58 @@
         <v>1</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>158</v>
+        <v>214</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="101.25" x14ac:dyDescent="0.2">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>166</v>
+        <v>217</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C35" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D35" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>171</v>
+        <v>218</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="J35" s="1" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="101.25" x14ac:dyDescent="0.2">
+        <v>218</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>167</v>
+        <v>234</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C36" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D36" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="J36" s="1" t="s">
-        <v>177</v>
+        <v>231</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>173</v>
+        <v>235</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>11</v>
@@ -2847,15 +2925,15 @@
         <v>1</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>171</v>
+        <v>233</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>175</v>
+        <v>241</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>174</v>
+        <v>236</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>11</v>
@@ -2867,317 +2945,335 @@
         <v>1</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>172</v>
+        <v>232</v>
       </c>
       <c r="I38" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39" s="4">
+        <v>0</v>
+      </c>
+      <c r="D39" s="4">
+        <v>1</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" s="4">
+        <v>0</v>
+      </c>
+      <c r="D40" s="4">
+        <v>1</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" s="4">
+        <v>1</v>
+      </c>
+      <c r="D41" s="4">
+        <v>0</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42" s="4">
+        <v>1</v>
+      </c>
+      <c r="D42" s="4">
+        <v>0</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="67.5" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C43" s="4">
+        <v>1</v>
+      </c>
+      <c r="D43" s="4">
+        <v>0</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="78.75" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44" s="4">
+        <v>1</v>
+      </c>
+      <c r="D44" s="4">
+        <v>0</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="56.25" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C45" s="4">
+        <v>1</v>
+      </c>
+      <c r="D45" s="4">
+        <v>0</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="56.25" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C46" s="4">
+        <v>1</v>
+      </c>
+      <c r="D46" s="4">
+        <v>0</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="135" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C47" s="4">
+        <v>1</v>
+      </c>
+      <c r="D47" s="4">
+        <v>0</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="101.25" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C48" s="4">
+        <v>1</v>
+      </c>
+      <c r="D48" s="4">
+        <v>0</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="101.25" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C49" s="4">
+        <v>1</v>
+      </c>
+      <c r="D49" s="4">
+        <v>0</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="J49" s="1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="56.25" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
+    <row r="50" spans="1:10" ht="101.25" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C50" s="4">
+        <v>1</v>
+      </c>
+      <c r="D50" s="4">
+        <v>0</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="56.25" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C51" s="4">
+        <v>1</v>
+      </c>
+      <c r="D51" s="4">
+        <v>0</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="G51" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="B39" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C39" s="4">
-        <v>1</v>
-      </c>
-      <c r="D39" s="4">
-        <v>0</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="G39" s="1" t="s">
+      <c r="H51" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="H39" s="1" t="s">
+      <c r="J51" s="1" t="s">
         <v>180</v>
-      </c>
-      <c r="J39" s="1" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="67.5" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C40" s="4">
-        <v>1</v>
-      </c>
-      <c r="D40" s="4">
-        <v>0</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="J40" s="1" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" ht="135" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C41" s="4">
-        <v>1</v>
-      </c>
-      <c r="D41" s="4">
-        <v>0</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="J41" s="1" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="67.5" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C42" s="4">
-        <v>1</v>
-      </c>
-      <c r="D42" s="4">
-        <v>0</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="J42" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C43" s="4">
-        <v>0</v>
-      </c>
-      <c r="D43" s="4">
-        <v>1</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="I43" s="1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C44" s="4">
-        <v>0</v>
-      </c>
-      <c r="D44" s="4">
-        <v>1</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="I44" s="1" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C45" s="4">
-        <v>0</v>
-      </c>
-      <c r="D45" s="4">
-        <v>1</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="I45" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" ht="67.5" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C46" s="4">
-        <v>1</v>
-      </c>
-      <c r="D46" s="4">
-        <v>0</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="J46" s="1" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C47" s="4">
-        <v>0</v>
-      </c>
-      <c r="D47" s="4">
-        <v>1</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="I47" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" ht="56.25" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C48" s="4">
-        <v>1</v>
-      </c>
-      <c r="D48" s="4">
-        <v>0</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="H48" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="J48" s="1" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C49" s="4">
-        <v>0</v>
-      </c>
-      <c r="D49" s="4">
-        <v>1</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="I49" s="1" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" ht="56.25" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C50" s="4">
-        <v>1</v>
-      </c>
-      <c r="D50" s="4">
-        <v>0</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="H50" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="J50" s="1" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A51" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C51" s="4">
-        <v>0</v>
-      </c>
-      <c r="D51" s="4">
-        <v>1</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="I51" s="1" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="67.5" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>217</v>
+        <v>181</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>11</v>
@@ -3189,200 +3285,564 @@
         <v>0</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>219</v>
+        <v>188</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>219</v>
+        <v>190</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>227</v>
+        <v>199</v>
       </c>
       <c r="J52" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="135" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C53" s="4">
+        <v>1</v>
+      </c>
+      <c r="D53" s="4">
+        <v>0</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="J53" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="67.5" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C54" s="4">
+        <v>1</v>
+      </c>
+      <c r="D54" s="4">
+        <v>0</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="J54" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" ht="67.5" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C55" s="4">
+        <v>1</v>
+      </c>
+      <c r="D55" s="4">
+        <v>0</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="J55" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="56.25" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C56" s="4">
+        <v>1</v>
+      </c>
+      <c r="D56" s="4">
+        <v>0</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="H56" s="1" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A53" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C53" s="4">
-        <v>0</v>
-      </c>
-      <c r="D53" s="4">
-        <v>1</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="I53" s="1" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" ht="45" x14ac:dyDescent="0.2">
-      <c r="A54" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C54" s="4">
-        <v>1</v>
-      </c>
-      <c r="D54" s="4">
-        <v>0</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="G54" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="H54" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="J54" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A55" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="B55" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C55" s="4">
-        <v>1</v>
-      </c>
-      <c r="D55" s="4">
-        <v>0</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="G55" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="H55" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" ht="45" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C56" s="4">
-        <v>1</v>
-      </c>
-      <c r="D56" s="4">
-        <v>0</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="G56" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="H56" s="1" t="s">
-        <v>75</v>
+      <c r="J56" s="1" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C57" s="4">
+        <v>1</v>
+      </c>
+      <c r="D57" s="4">
+        <v>0</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" ht="67.5" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C58" s="4">
+        <v>1</v>
+      </c>
+      <c r="D58" s="4">
+        <v>0</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="J58" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C59" s="4">
+        <v>1</v>
+      </c>
+      <c r="D59" s="4">
+        <v>0</v>
+      </c>
+      <c r="E59" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="B57" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C57" s="4">
-        <v>1</v>
-      </c>
-      <c r="D57" s="4">
-        <v>0</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="G57" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="H57" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="J57" s="1" t="s">
+      <c r="G59" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="J59" s="1" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A58" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C58" s="4">
-        <v>0</v>
-      </c>
-      <c r="D58" s="4">
-        <v>1</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="I58" s="1" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A59" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C59" s="4">
-        <v>0</v>
-      </c>
-      <c r="D59" s="4">
-        <v>1</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="I59" s="1" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:10" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="B60" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C60" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D60" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="I60" s="1" t="s">
+      <c r="G60" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C61" s="4">
+        <v>1</v>
+      </c>
+      <c r="D61" s="4">
+        <v>0</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" ht="56.25" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C62" s="4">
+        <v>1</v>
+      </c>
+      <c r="D62" s="4">
+        <v>0</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="J62" s="1" t="s">
         <v>243</v>
       </c>
     </row>
+    <row r="63" spans="1:10" ht="90" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C63" s="4">
+        <v>1</v>
+      </c>
+      <c r="D63" s="4">
+        <v>0</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="J63" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" ht="112.5" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C64" s="4">
+        <v>1</v>
+      </c>
+      <c r="D64" s="4">
+        <v>0</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="J64" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" ht="101.25" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C65" s="4">
+        <v>1</v>
+      </c>
+      <c r="D65" s="4">
+        <v>0</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="J65" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="112.5" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C66" s="4">
+        <v>1</v>
+      </c>
+      <c r="D66" s="4">
+        <v>0</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="J66" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" ht="90" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C67" s="4">
+        <v>1</v>
+      </c>
+      <c r="D67" s="4">
+        <v>0</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="J67" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" ht="123.75" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C68" s="4">
+        <v>1</v>
+      </c>
+      <c r="D68" s="4">
+        <v>0</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="J68" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" ht="168.75" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C69" s="4">
+        <v>1</v>
+      </c>
+      <c r="D69" s="4">
+        <v>0</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="J69" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" ht="135" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C70" s="4">
+        <v>1</v>
+      </c>
+      <c r="D70" s="4">
+        <v>0</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="J70" s="1" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C71" s="4">
+        <v>0</v>
+      </c>
+      <c r="D71" s="4">
+        <v>1</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="I71" s="1" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C72" s="4">
+        <v>0</v>
+      </c>
+      <c r="D72" s="4">
+        <v>1</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="I72" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C73" s="4">
+        <v>0</v>
+      </c>
+      <c r="D73" s="4">
+        <v>1</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="I73" s="1" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C74" s="4">
+        <v>0</v>
+      </c>
+      <c r="D74" s="4">
+        <v>1</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="I74" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A22:J64">
+    <sortCondition ref="C22:C64"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Complete Templating for Symptom Property Questions
</commit_message>
<xml_diff>
--- a/intent-definition.xlsx
+++ b/intent-definition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\User\Documents\Code\Thesis\Symptom-Checker-Chatbot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{188B5497-9CC8-4783-8BEC-D2F7B0054AD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6182BB9-2FBA-41F8-A986-2D3B410C20D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2107,8 +2107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{563BB99E-AECF-4E9F-90DC-16BA1EB2C1A9}">
   <dimension ref="A1:M74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I73" sqref="I73"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Updated moisture property to cover (Damp, Drenched) for hyperhidrosis. Added Painkillers property. Added Triage function. Added Visibility property.
</commit_message>
<xml_diff>
--- a/intent-definition.xlsx
+++ b/intent-definition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\User\Documents\Code\Thesis\Symptom-Checker-Chatbot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6182BB9-2FBA-41F8-A986-2D3B410C20D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5627051-C722-42D4-95D1-3071E0EFD472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="305">
   <si>
     <t>parameters</t>
   </si>
@@ -901,6 +901,42 @@
   </si>
   <si>
     <t>respiratory_set</t>
+  </si>
+  <si>
+    <t>pain_killers_yes</t>
+  </si>
+  <si>
+    <t>pain_killers_no</t>
+  </si>
+  <si>
+    <t>fallback_pain_killers</t>
+  </si>
+  <si>
+    <t>PAINKILLER</t>
+  </si>
+  <si>
+    <t>Again does pain killers work?</t>
+  </si>
+  <si>
+    <t>visibility_set</t>
+  </si>
+  <si>
+    <t>fallback_visibility</t>
+  </si>
+  <si>
+    <t>VISIBILITY</t>
+  </si>
+  <si>
+    <t>{@visibility:$visibility:1:0}</t>
+  </si>
+  <si>
+    <t>PAINKILLERS</t>
+  </si>
+  <si>
+    <t>{@visibility:cloudy}|It is {@visibility:clear}|It looks {@visibility:murky}|I see it as {@visibility:clear}|very {@visibility:clear}|about {@visibility:clear}|around {@visibility:clear}</t>
+  </si>
+  <si>
+    <t>Again how does it look?</t>
   </si>
 </sst>
 </file>
@@ -2105,10 +2141,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{563BB99E-AECF-4E9F-90DC-16BA1EB2C1A9}">
-  <dimension ref="A1:M74"/>
+  <dimension ref="A1:M79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H78" sqref="H78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -3837,6 +3873,109 @@
       </c>
       <c r="I74" s="1" t="s">
         <v>279</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C75" s="4">
+        <v>1</v>
+      </c>
+      <c r="D75" s="4">
+        <v>0</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="H75" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C76" s="4">
+        <v>1</v>
+      </c>
+      <c r="D76" s="4">
+        <v>0</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="H76" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C77" s="4">
+        <v>0</v>
+      </c>
+      <c r="D77" s="4">
+        <v>1</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="I77" s="1" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" ht="78.75" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C78" s="4">
+        <v>1</v>
+      </c>
+      <c r="D78" s="4">
+        <v>0</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="H78" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="J78" s="1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C79" s="4">
+        <v>0</v>
+      </c>
+      <c r="D79" s="4">
+        <v>1</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="I79" s="1" t="s">
+        <v>304</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Update Intent functionality [IntentManager] Added Tagalog Intents
</commit_message>
<xml_diff>
--- a/intent-definition.xlsx
+++ b/intent-definition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\User\Documents\Code\Thesis\Symptom-Checker-Chatbot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5627051-C722-42D4-95D1-3071E0EFD472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{350A6856-C9FB-46A1-94D7-4026C2BFFBD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="base" sheetId="11" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="373">
   <si>
     <t>parameters</t>
   </si>
@@ -216,15 +216,9 @@
     <t>checkup</t>
   </si>
   <si>
-    <t>Hi,Magandang  umaga,Kamusta,Magandang gabi,Hello</t>
-  </si>
-  <si>
     <t>Hello|Hi|Hey|What's up|Good morning</t>
   </si>
   <si>
-    <t>Check up|Evaluate me|Examine me|Test me|Help me</t>
-  </si>
-  <si>
     <t>Yes|Okay I will|Why not|Yes that's alright|Yes I do|Exactly|Of course|Yep that's ok|Okay|Ok</t>
   </si>
   <si>
@@ -912,9 +906,6 @@
     <t>fallback_pain_killers</t>
   </si>
   <si>
-    <t>PAINKILLER</t>
-  </si>
-  <si>
     <t>Again does pain killers work?</t>
   </si>
   <si>
@@ -937,6 +928,222 @@
   </si>
   <si>
     <t>Again how does it look?</t>
+  </si>
+  <si>
+    <t>Hello|Hi|Kamusta|Magandang Umaga|Kumusta|Musta|Pre|Hai</t>
+  </si>
+  <si>
+    <t>Suriin|Suriin ako|Subukan ako|Tulungan ako|Check up|Checkup|Patingin ako</t>
+  </si>
+  <si>
+    <t>Oo|Sige gagawin ko|Bakit hindi|Oo okay lang|Oo gagawin ko|Eksakto|Siyempre|Oo ok lang|Okay|Ok</t>
+  </si>
+  <si>
+    <t>No way|Hindi|Na|Hindi ko kaya|Hindi ko kaya|Huwag|Hindi|Hindi ako sumasang-ayon|Siyempre hindi|Hindi salamat|Hindi ngayon|Nah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+{@language:english}|Gusto ko ng {@language:tagalog}|Piliin ko ang {@language:filipino}|{@language:english} please|Sabay tayo sa {@language:tagalog}|Palitan ito ng {@language: filipino}|Gumamit ng {@language:filipino} sa halip</t>
+  </si>
+  <si>
+    <t>Gusto kong baguhin ang aking wika|Hayaan akong magpalit ng wika|Baguhin ang wika|Palitan ang aking wika sa {@language:english}|Gamitin ang {@language:english} sa halip</t>
+  </si>
+  <si>
+    <t>Paumanhin, mangyaring sagutin ang tanong. Sumasang-ayon ka ba sa aking mga tuntunin ng serbisyo?|Paumanhin? Sumasang-ayon ka ba sa aking mga tuntunin ng serbisyo?</t>
+  </si>
+  <si>
+    <t>Anong wika?|Paumanhin, hindi ko masyadong naintindihan. Anong wika ang gusto mo?</t>
+  </si>
+  <si>
+    <t>Check up|Evaluate me|Examine me|Test me|Help me|Checkup</t>
+  </si>
+  <si>
+    <t>Ako ay {@sys.age:20} taong gulang|{@sys.age:30} taong gulang|Ako ay {@sys.age:30} taong gulang ngayon|{@sys.age:25} gulang| {@sys.age:18} taon</t>
+  </si>
+  <si>
+    <t>{@sex:lalaki}|Ako ay isang {@sex:babae}|Ako ay isang {@sex:lalaki}|Ang aking kasarian ay {@sex:babae}|Ang aking kasarian ay {@sex:lalaki}</t>
+  </si>
+  <si>
+    <t>Ulit ilang taon ka na?|Hindi ko nakuha yan, anong edad mo?</t>
+  </si>
+  <si>
+    <t>Anong pangalan?</t>
+  </si>
+  <si>
+    <t>Anong kasarian?|Ano ang iyong biological sex?</t>
+  </si>
+  <si>
+    <t>{@symptom:ubo}|Nagkaroon ng {@symptom:ubo}|Naghihirap mula sa {@symptom:ubo}|Nakararamdam ng {@symptom:lagnat}|Itong patuloy na {@symptom:lagnat }|Itong {@symptom:hilo}|Pakikitungo sa {@symptom:ubo}|Pababa sa {@symptom:ubo}|Pakikipagpunyagi sa isang {@symptom:lagnat}|Nakontrata ng {@symptom:lagnat}|Patuloy na {@symptom:ubo}|Ma{@symptom:ubo}|Um{@symptom:ubo}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Anong sintomas?|Maaari mo bang ibahagi ang isang sintomas?</t>
+  </si>
+  <si>
+    <t>Meron ka ulit?</t>
+  </si>
+  <si>
+    <t>Gaano katagal ulit?</t>
+  </si>
+  <si>
+    <t>Muli gaano kabigat?</t>
+  </si>
+  <si>
+    <t>Muli, ano ang iyong temperatura?</t>
+  </si>
+  <si>
+    <t>Gaano kadalas ulit?</t>
+  </si>
+  <si>
+    <t>Muli gaano kasakit?</t>
+  </si>
+  <si>
+    <t>Muli gaano mahina?</t>
+  </si>
+  <si>
+    <t>Aling mata na naman?</t>
+  </si>
+  <si>
+    <t>Muli anong bahagi ng katawan?</t>
+  </si>
+  <si>
+    <t>Muli, ito ba ay pangkalahatan o naisalokal?</t>
+  </si>
+  <si>
+    <t>Ano ulit ang kulay?</t>
+  </si>
+  <si>
+    <t>Muli gaano kahirap?</t>
+  </si>
+  <si>
+    <t>Muli, ito ba ay tuyo o basa?</t>
+  </si>
+  <si>
+    <t>Muli, ito ba ay nagpapahinga o sa panahon ng aktibidad?</t>
+  </si>
+  <si>
+    <t>Ulit ilang beses?</t>
+  </si>
+  <si>
+    <t>Nakialam ba ito?</t>
+  </si>
+  <si>
+    <t>Anong oras ng araw?</t>
+  </si>
+  <si>
+    <t>Muli, ano ang iyong tibok ng puso? (x bpm)</t>
+  </si>
+  <si>
+    <t>Muli, ano ang iyong presyon ng dugo? x/y</t>
+  </si>
+  <si>
+    <t>Oo|Sige gagawin ko|Bakit hindi|Oo ayos lang|Oo kaya ko|Eksakto|Siyempre|Oo ok lang|Okay|Ok|Meron ako</t>
+  </si>
+  <si>
+    <t>No way|Hindi|Na|Hindi ko kaya|Hindi ko kaya|Huwag|Hindi|Hindi ako sumasang-ayon|Siyempre hindi|Hindi salamat|Hindi ngayon|Nah|Wala ako|Wala ito</t>
+  </si>
+  <si>
+    <t>{@duration_generic:Ilang araw}|Nakuha ko ito sa loob ng {@duration_generic:ilang linggo}|Isang mag-asawa {@duration_generic:araw}|Tungkol sa isang {@duration_generic:araw}|Hanggang isang {@duration_generic:Buwan}</t>
+  </si>
+  <si>
+    <t>{@sys.duration:2 days}|Naging {@sys.duration:3 days}|Mga {@sys.duration:4 days}|Mga {@sys.duration:5 days}|Nakuha ko ito nang {@sys.duration:5 araw}|{@sys.duration:5 days} ang lumipas|Isang {@sys.duration:1 month}</t>
+  </si>
+  <si>
+    <t>{@sys.unit-weight: 60kg}|Ako ay {@sys.unit-weight: 60kg}|Tumitimbang ako ng {@sys.unit-weight: 60kg}|Mga {@sys.unit-weight: 60kg}|Siguro mga {@sys.unit-weight: 60kg}</t>
+  </si>
+  <si>
+    <t>{@sys.duration:2 days}|Mayroon ako nito sa loob ng {@sys.duration:2 weeks} ngayon|Tungkol sa {@sys.duration:2 weeks}|Mga {@sys.duration:3 weeks}|Nakuha ko ito nang {@sys.duration:2 weeks}|Nangyari ito sa loob ng {@sys.duration:2 weeks}|{@sys.duration:2 linggo} ang haba|Bawat {@sys.duration:2 weeks}</t>
+  </si>
+  <si>
+    <t>{@frequency_adverbs:minsan}|{@frequency_adverbs:madalas} kapag|Nangyayari ito {@frequency_adverbs:lingguhan}|Meron ako nito {@frequency_adverbs:araw-araw}|Napaka {@frequency_adverbs:madalas}|{@frequency_adverbs:minsan} |Ito ay nangyayari {@frequency_adverbs:minsan}|Nakukuha ito {@frequency_adverbs:minsan}</t>
+  </si>
+  <si>
+    <t>{@intensity:1}|Sa paligid ng {@intensity:2}|Binibigyan ko ito ng {@intensity:3}|Isang sukat ng {@intensity:4}|Isang intensity ng {@intensity:5}|Sa tingin ko ito ay isang {@intensity:6}|{@intensity:7} malakas|{@intensity:8} mahina|Level {@intensity:9}|Tinatayang {@intensity:10}</t>
+  </si>
+  <si>
+    <t>{@pain_adjectives:hapdi}|Ma{@pain_adjectives:hapdi}|Nararamdaman ko ang {@pain_adjectives:tinding} sakit|Nararamdaman ko ang ma{@pain_adjectives:tinding} sakit|Ito ay {@pain_adjectives:sakit}|Ito ay ma{@pain_adjectives:sakit}|</t>
+  </si>
+  <si>
+    <t>{@location_body_locale:ulo}|Aking {@location_body_locale:likod}|Nararamdaman ko ito sa aking {@location_body_locale:tenga}|Sa aking {@location_body_locale:paa}|Masakit sa aking {@location_body_locale:binti}|Sa paligid ng aking { @location_body_locale:dibdib} area|{@location_body_locale:braso} area</t>
+  </si>
+  <si>
+    <t>{@location_body_region:localized}|Ito ay {@location_body_region:localized}|Sa {@location_body_region:localized} na rehiyon</t>
+  </si>
+  <si>
+    <t>{@color_phlegm:berde}|Ma{@color_phlegm:berde}|Ito ay kulay {@color_phlegm:putik}|Kulay {@color_phlegm:berde}|Kulay ma{@color_phlegm:berde}|Ito ay {@color_phlegm:puti}|Ito ay ma{@color_phlegm:puti}|Ito ay mukhang {@color_phlegm:dilaw}|Ito ay mukhang ma{@color_phlegm:dilaw}|may {@color_phlegm:berde} kulay</t>
+  </si>
+  <si>
+    <t>{@difficulty:dali}|Ma{@difficulty:dali}|Ito ay {@difficulty:easy}|Ito ay ma{@difficulty:hirap}|Sa tingin ko ay {@difficulty:dali}|Sa tingin ko ay ma{@difficulty:dali}|Napaka {@difficulty:dali}|Basta {@difficulty:mahirap}</t>
+  </si>
+  <si>
+    <t>{@moisture:basa}|ma{@moisture:basa}|Ito ay {@moisture:basang-basa}|Ito ay ma{@moisture:basa}|Napaka {@moisture:tuyo}|Napaka ma{@moisture:tuyo}|Nararamdaman ko {@moisture:basa}|Nararamdaman ko ma{@moisture:basa}|Basta {@moisture:basa}</t>
+  </si>
+  <si>
+    <t>{@sys.number:2}|{@sys.number:2} beses|Mga {@sys.number:2} beses|Higit sa {@sys.number:2} beses|{@sys.number:2} na</t>
+  </si>
+  <si>
+    <t>{@physical_state:rest}|Ma{@physical_state:rest}|Nag{@physical_state:rest}|Sa panahon ng {@physical_state:trabaho}|Sa {@physical_state:rest}|Ito ay nangyayari sa panahon ng {@physical_state:rest}|Ito ay nangyayari sa panahon ng nag{@physical_state:rest}|Habang nag{@physical_state:rest}Habang {@physical_state:trabaho}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+No way|Hindi|Na|Hindi ko kaya|Hindi ko kaya|Huwag|Hindi|Hindi ako sumasang-ayon|Siyempre hindi|Hindi salamat|Hindi ngayon|Nah</t>
+  </si>
+  <si>
+    <t>{@heartrate:120}|{@heartrate:90} bpm|{@heartrate:40} beats|{@heartrate:79} beats kada minuto|My heartrate is {@heartrate:88}|Heartrate of {@heartrate:111 }|Rate ng {@heartrate:120}|Ito ay {@heartrate:80}</t>
+  </si>
+  <si>
+    <t>{@trigger_activity:walking}|sa panahon ng {@trigger_activity:walking}|habang {@trigger_activity:walking}|naganap noong {@trigger_activity:walking}|trigger ng {@trigger_activity:walking}|ng {@trigger_activity:walking}|sanhi ni {@trigger_activity:walking}|Ako ay {@trigger_activity:walking}</t>
+  </si>
+  <si>
+    <t>{@trigger_state:stressed}|Noong {@trigger_state:stressed}|ako ay {@trigger_state:stressed}|sa panahon ng {@trigger_state:stressed}|ako ay {@trigger_state:stressed}|nadama {@trigger_state:stressed}|ay {@trigger_state:stressed}|{@trigger_state:stressed} ang nag-trigger nito|nangyari noong ako ay {@trigger_state:stressed}</t>
+  </si>
+  <si>
+    <t>{@trigger_food:milk}|pagkain ng {@trigger_food:milk}|pag-inom ng {@trigger_food:milk}|pag-inom ng {@trigger_food:milk}|noong nagkaroon ako ng {@trigger_food:milk}|kumain ng {@trigger_food:milk}|{@trigger_food:milk}|sinubukan ang {@trigger_food:milk}</t>
+  </si>
+  <si>
+    <t>Muli, ano ang hitsura nito?</t>
+  </si>
+  <si>
+    <t>Muli gumagana ang mga pain killer?</t>
+  </si>
+  <si>
+    <t>Muli, ano ang nag-trigger nito?</t>
+  </si>
+  <si>
+    <t>Muli may pagbabago ba?</t>
+  </si>
+  <si>
+    <t>Muli ang anumang kasaysayan na may sakit na cardiovascular?</t>
+  </si>
+  <si>
+    <t>Muli ang anumang kasaysayan na may sakit sa paghinga?</t>
+  </si>
+  <si>
+    <t>{@cardiovascular:heart failure}|Ako ay nagkaroon ng {@cardiovascular:heart failure}|Ang aking pamilya ay nagkaroon ng {@cardiovascular:heart failure}|may history sa {@cardiovascular:heart failure}|Ang aking ina ay may {@cardiovascular:heart failure }|May {@cardiovascular:heart failure} ang side ng tatay ko|May history kami ng {@cardiovascular:heart failure}|Nagkaroon ako ng {@cardiovascular:heart failure}|nagkaroon ng {@cardiovascular:heart failure}</t>
+  </si>
+  <si>
+    <t>{@respiratory:asthma}|Nagkaroon ako ng {@respiratory:asthma}|Ang aking pamilya ay nagkaroon ng {@respiratory:asthma}|may history sa {@respiratory:asthma}|Ang aking ina ay may {@respiratory:asthma}|Ang aking ama sa panig may {@respiratory:asthma}|May history kami ng {@respiratory:asthma}|Nagkaroon ako ng {@respiratory:asthma}|may {@respiratory:asthma}</t>
+  </si>
+  <si>
+    <t>{@change_quantity:increase}|ito ay {@change_quantity:increase}|may {@change_quantity:increase}|may {@change_quantity:increase}|Napansin kong {@change_quantity:increase}|unti-unti {@change_quantity:increase}| ay {@change_quantity:increase}|ito ay {@change_quantity:increase}</t>
+  </si>
+  <si>
+    <t>{@visibility:cloudy}|Ma{@visibility:cloudy}|Ito ay {@visibility:clear}|Ito ay ma{@visibility:clear}|Mukhang {@visibility:murky}|Mukhang ma{@visibility:murky}|Nakikita ko ito bilang {@visibility:clear}|Nakikita ko ito bilang na{@visibility:clear}|napaka {@visibility:clear}|tungkol sa {@visibility:clear }|sa paligid ng {@visibility:clear}</t>
+  </si>
+  <si>
+    <t>{@sys.temperature: 38°}|Ang katawan ko ay {@sys.temperature: 38C}|Sa paligid ng {@sys.temperature: 38°}|Tungkol sa {@sys.temperature: 38C}|Ito ay {@sys.temperature: 38 degrees}</t>
+  </si>
+  <si>
+    <t>{@location_eyes:left}|Ang {@location_eyes:kawliwa} na mata|Ito ay nasa {@location_eyes:kaliwa}|{@location_eyes:pareho} na mga mata|Aking {@location_eyes:kanan} na mata|Nararamdaman ko ito sa aking {@location_eyes:kaliwa} mata</t>
+  </si>
+  <si>
+    <t>{@blood_pressure:120/90}|Ang presyon ng dugo ko ay {@blood_pressure:30/90}|Ito ay {@blood_pressure:110/80}|Ang BP ko ay {@blood_pressure:25/44}|Sinusukat nito ang {@blood_pressure:77/91}|Sa paligid ng {@blood_pressure:112/94}|Tungkol sa {@blood_pressure:140/93}|Mga antas ito ng {@blood_pressure:130/78}</t>
+  </si>
+  <si>
+    <t>{@sys.any:Steven}|Maaari mo akong tawagan {@sys.any:Mark}|Tugunan ako bilang {@sys.any:Robert}|Ang pangalan ko ay {@sys.any:Maxson}|Tawagan ako {@sys.any:Roy}</t>
+  </si>
+  <si>
+    <t>{@parts_day:umaga}|Madaling {@parts_day:umaga}|Sa {@parts_day:gabi}|Sa {@parts_day:almusal}|sa panahon ng {@parts_day:gabi}|sa paligid ng {@parts_day:hapon}</t>
   </si>
 </sst>
 </file>
@@ -1456,7 +1663,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1470,6 +1677,9 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -2143,8 +2353,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{563BB99E-AECF-4E9F-90DC-16BA1EB2C1A9}">
   <dimension ref="A1:M79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H78" sqref="H78"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -2217,10 +2427,10 @@
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="22.5" x14ac:dyDescent="0.2">
@@ -2237,15 +2447,15 @@
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>66</v>
+        <v>310</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>11</v>
@@ -2257,18 +2467,18 @@
         <v>0</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="45" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>11</v>
@@ -2280,18 +2490,18 @@
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="78.75" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>11</v>
@@ -2303,21 +2513,21 @@
         <v>0</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>11</v>
@@ -2329,13 +2539,13 @@
         <v>0</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>15</v>
@@ -2343,7 +2553,7 @@
     </row>
     <row r="8" spans="1:13" ht="45" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>11</v>
@@ -2355,15 +2565,15 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>11</v>
@@ -2375,15 +2585,15 @@
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>11</v>
@@ -2395,12 +2605,12 @@
         <v>0</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>11</v>
@@ -2412,21 +2622,21 @@
         <v>0</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>11</v>
@@ -2438,21 +2648,21 @@
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="45" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>11</v>
@@ -2464,21 +2674,21 @@
         <v>0</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>11</v>
@@ -2490,15 +2700,15 @@
         <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>11</v>
@@ -2510,15 +2720,15 @@
         <v>1</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>11</v>
@@ -2530,15 +2740,15 @@
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="135" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>11</v>
@@ -2550,23 +2760,23 @@
         <v>0</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I17" s="4"/>
       <c r="J17" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="K17" s="4"/>
     </row>
     <row r="18" spans="1:11" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>11</v>
@@ -2578,15 +2788,15 @@
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>11</v>
@@ -2598,55 +2808,55 @@
         <v>0</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="4">
+        <v>1</v>
+      </c>
+      <c r="D20" s="4">
+        <v>0</v>
+      </c>
+      <c r="H20" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" s="4">
-        <v>1</v>
-      </c>
-      <c r="D20" s="4">
-        <v>0</v>
-      </c>
-      <c r="H20" s="1" t="s">
+      <c r="J20" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="4">
+        <v>1</v>
+      </c>
+      <c r="D21" s="4">
+        <v>0</v>
+      </c>
+      <c r="H21" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="4">
-        <v>1</v>
-      </c>
-      <c r="D21" s="4">
-        <v>0</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>139</v>
-      </c>
       <c r="J21" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>11</v>
@@ -2658,15 +2868,15 @@
         <v>1</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>11</v>
@@ -2678,15 +2888,15 @@
         <v>1</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>11</v>
@@ -2698,15 +2908,15 @@
         <v>1</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>11</v>
@@ -2718,15 +2928,15 @@
         <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>11</v>
@@ -2738,55 +2948,55 @@
         <v>1</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="4">
+        <v>0</v>
+      </c>
+      <c r="D27" s="4">
+        <v>1</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="I27" s="1" t="s">
         <v>172</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C27" s="4">
-        <v>0</v>
-      </c>
-      <c r="D27" s="4">
-        <v>1</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="4">
+        <v>0</v>
+      </c>
+      <c r="D28" s="4">
+        <v>1</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="I28" s="1" t="s">
         <v>173</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C28" s="4">
-        <v>0</v>
-      </c>
-      <c r="D28" s="4">
-        <v>1</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>11</v>
@@ -2798,35 +3008,35 @@
         <v>1</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="4">
+        <v>0</v>
+      </c>
+      <c r="D30" s="4">
+        <v>1</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="B30" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C30" s="4">
-        <v>0</v>
-      </c>
-      <c r="D30" s="4">
-        <v>1</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>187</v>
-      </c>
       <c r="I30" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>11</v>
@@ -2838,98 +3048,98 @@
         <v>1</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" s="4">
+        <v>0</v>
+      </c>
+      <c r="D32" s="4">
+        <v>1</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="I32" s="1" t="s">
         <v>204</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C32" s="4">
-        <v>0</v>
-      </c>
-      <c r="D32" s="4">
-        <v>1</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="4">
+        <v>0</v>
+      </c>
+      <c r="D33" s="4">
+        <v>1</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="I33" s="1" t="s">
         <v>209</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C33" s="4">
-        <v>0</v>
-      </c>
-      <c r="D33" s="4">
-        <v>1</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" s="4">
+        <v>0</v>
+      </c>
+      <c r="D34" s="4">
+        <v>1</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="I34" s="1" t="s">
         <v>213</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C34" s="4">
-        <v>0</v>
-      </c>
-      <c r="D34" s="4">
-        <v>1</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="I34" s="1" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" s="4">
+        <v>0</v>
+      </c>
+      <c r="D35" s="4">
+        <v>1</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="I35" s="1" t="s">
         <v>217</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C35" s="4">
-        <v>0</v>
-      </c>
-      <c r="D35" s="4">
-        <v>1</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="I35" s="1" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>11</v>
@@ -2941,15 +3151,15 @@
         <v>1</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>11</v>
@@ -2961,15 +3171,15 @@
         <v>1</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>11</v>
@@ -2981,15 +3191,15 @@
         <v>1</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>11</v>
@@ -3001,15 +3211,15 @@
         <v>1</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>11</v>
@@ -3021,61 +3231,61 @@
         <v>1</v>
       </c>
       <c r="E40" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="I40" s="1" t="s">
         <v>252</v>
-      </c>
-      <c r="I40" s="1" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" s="4">
+        <v>1</v>
+      </c>
+      <c r="D41" s="4">
+        <v>0</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G41" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B41" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C41" s="4">
-        <v>1</v>
-      </c>
-      <c r="D41" s="4">
-        <v>0</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>119</v>
-      </c>
       <c r="H41" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42" s="4">
+        <v>1</v>
+      </c>
+      <c r="D42" s="4">
+        <v>0</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G42" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B42" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C42" s="4">
-        <v>1</v>
-      </c>
-      <c r="D42" s="4">
-        <v>0</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>120</v>
-      </c>
       <c r="H42" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="67.5" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>11</v>
@@ -3087,21 +3297,21 @@
         <v>0</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="78.75" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>11</v>
@@ -3113,21 +3323,21 @@
         <v>0</v>
       </c>
       <c r="E44" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G44" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="G44" s="1" t="s">
-        <v>123</v>
-      </c>
       <c r="H44" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>11</v>
@@ -3139,47 +3349,47 @@
         <v>0</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C46" s="4">
+        <v>1</v>
+      </c>
+      <c r="D46" s="4">
+        <v>0</v>
+      </c>
+      <c r="E46" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B46" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C46" s="4">
-        <v>1</v>
-      </c>
-      <c r="D46" s="4">
-        <v>0</v>
-      </c>
-      <c r="E46" s="1" t="s">
+      <c r="G46" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="G46" s="1" t="s">
-        <v>148</v>
-      </c>
       <c r="H46" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="135" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>11</v>
@@ -3191,125 +3401,125 @@
         <v>0</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="101.25" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C48" s="4">
+        <v>1</v>
+      </c>
+      <c r="D48" s="4">
+        <v>0</v>
+      </c>
+      <c r="E48" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B48" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C48" s="4">
-        <v>1</v>
-      </c>
-      <c r="D48" s="4">
-        <v>0</v>
-      </c>
-      <c r="E48" s="1" t="s">
+      <c r="G48" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="G48" s="1" t="s">
-        <v>159</v>
-      </c>
       <c r="H48" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="101.25" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C49" s="4">
+        <v>1</v>
+      </c>
+      <c r="D49" s="4">
+        <v>0</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G49" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B49" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C49" s="4">
-        <v>1</v>
-      </c>
-      <c r="D49" s="4">
-        <v>0</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="G49" s="1" t="s">
+      <c r="H49" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="H49" s="1" t="s">
-        <v>169</v>
-      </c>
       <c r="J49" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="101.25" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C50" s="4">
+        <v>1</v>
+      </c>
+      <c r="D50" s="4">
+        <v>0</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G50" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B50" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C50" s="4">
-        <v>1</v>
-      </c>
-      <c r="D50" s="4">
-        <v>0</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>168</v>
-      </c>
       <c r="H50" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C51" s="4">
+        <v>1</v>
+      </c>
+      <c r="D51" s="4">
+        <v>0</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="H51" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="B51" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C51" s="4">
-        <v>1</v>
-      </c>
-      <c r="D51" s="4">
-        <v>0</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="G51" s="1" t="s">
+      <c r="J51" s="1" t="s">
         <v>178</v>
-      </c>
-      <c r="H51" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="J51" s="1" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="67.5" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>11</v>
@@ -3321,21 +3531,21 @@
         <v>0</v>
       </c>
       <c r="E52" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G52" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="G52" s="1" t="s">
-        <v>190</v>
-      </c>
       <c r="H52" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="135" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>11</v>
@@ -3347,21 +3557,21 @@
         <v>0</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="67.5" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>11</v>
@@ -3373,21 +3583,21 @@
         <v>0</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="67.5" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>11</v>
@@ -3399,99 +3609,99 @@
         <v>0</v>
       </c>
       <c r="E55" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="G55" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="G55" s="1" t="s">
+      <c r="H55" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="H55" s="1" t="s">
-        <v>207</v>
-      </c>
       <c r="J55" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C56" s="4">
+        <v>1</v>
+      </c>
+      <c r="D56" s="4">
+        <v>0</v>
+      </c>
+      <c r="E56" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="B56" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C56" s="4">
-        <v>1</v>
-      </c>
-      <c r="D56" s="4">
-        <v>0</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>210</v>
-      </c>
       <c r="G56" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C57" s="4">
+        <v>1</v>
+      </c>
+      <c r="D57" s="4">
+        <v>0</v>
+      </c>
+      <c r="E57" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B57" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C57" s="4">
-        <v>1</v>
-      </c>
-      <c r="D57" s="4">
-        <v>0</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>214</v>
-      </c>
       <c r="G57" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="58" spans="1:10" ht="67.5" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C58" s="4">
+        <v>1</v>
+      </c>
+      <c r="D58" s="4">
+        <v>0</v>
+      </c>
+      <c r="E58" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="B58" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C58" s="4">
-        <v>1</v>
-      </c>
-      <c r="D58" s="4">
-        <v>0</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>218</v>
-      </c>
       <c r="G58" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B59" s="4" t="s">
         <v>11</v>
@@ -3503,21 +3713,21 @@
         <v>0</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B60" s="4" t="s">
         <v>11</v>
@@ -3529,18 +3739,18 @@
         <v>0</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B61" s="4" t="s">
         <v>11</v>
@@ -3552,70 +3762,70 @@
         <v>0</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C62" s="4">
+        <v>1</v>
+      </c>
+      <c r="D62" s="4">
+        <v>0</v>
+      </c>
+      <c r="E62" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="B62" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C62" s="4">
-        <v>1</v>
-      </c>
-      <c r="D62" s="4">
-        <v>0</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>232</v>
-      </c>
       <c r="G62" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="J62" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="90" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C63" s="4">
+        <v>1</v>
+      </c>
+      <c r="D63" s="4">
+        <v>0</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="J63" s="1" t="s">
         <v>248</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C63" s="4">
-        <v>1</v>
-      </c>
-      <c r="D63" s="4">
-        <v>0</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="G63" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="H63" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="J63" s="1" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="112.5" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B64" s="4" t="s">
         <v>11</v>
@@ -3627,21 +3837,21 @@
         <v>0</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="101.25" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B65" s="4" t="s">
         <v>11</v>
@@ -3653,21 +3863,21 @@
         <v>0</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="J65" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="112.5" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B66" s="4" t="s">
         <v>11</v>
@@ -3679,21 +3889,21 @@
         <v>0</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="J66" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="90" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B67" s="4" t="s">
         <v>11</v>
@@ -3705,21 +3915,21 @@
         <v>0</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="J67" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="123.75" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B68" s="4" t="s">
         <v>11</v>
@@ -3731,21 +3941,21 @@
         <v>0</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="J68" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="168.75" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B69" s="4" t="s">
         <v>11</v>
@@ -3757,21 +3967,21 @@
         <v>0</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="135" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B70" s="4" t="s">
         <v>11</v>
@@ -3783,21 +3993,21 @@
         <v>0</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="J70" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B71" s="4" t="s">
         <v>11</v>
@@ -3809,35 +4019,35 @@
         <v>1</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C72" s="4">
+        <v>0</v>
+      </c>
+      <c r="D72" s="4">
+        <v>1</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="I72" s="1" t="s">
         <v>275</v>
-      </c>
-      <c r="B72" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C72" s="4">
-        <v>0</v>
-      </c>
-      <c r="D72" s="4">
-        <v>1</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="I72" s="1" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="73" spans="1:10" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B73" s="4" t="s">
         <v>11</v>
@@ -3849,15 +4059,15 @@
         <v>1</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="74" spans="1:10" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B74" s="4" t="s">
         <v>11</v>
@@ -3869,15 +4079,15 @@
         <v>1</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="75" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B75" s="4" t="s">
         <v>11</v>
@@ -3889,15 +4099,15 @@
         <v>0</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="76" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B76" s="4" t="s">
         <v>11</v>
@@ -3909,15 +4119,15 @@
         <v>0</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B77" s="4" t="s">
         <v>11</v>
@@ -3929,38 +4139,38 @@
         <v>1</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="78" spans="1:10" ht="78.75" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C78" s="4">
+        <v>1</v>
+      </c>
+      <c r="D78" s="4">
+        <v>0</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="H78" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="J78" s="1" t="s">
         <v>298</v>
-      </c>
-      <c r="B78" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C78" s="4">
-        <v>1</v>
-      </c>
-      <c r="D78" s="4">
-        <v>0</v>
-      </c>
-      <c r="G78" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="H78" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="J78" s="1" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B79" s="4" t="s">
         <v>11</v>
@@ -3972,10 +4182,10 @@
         <v>1</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
   </sheetData>
@@ -3989,10 +4199,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AF69D1E-B293-4AC9-BAA2-CC12BCEF0879}">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:M79"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H55" sqref="H55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -4002,7 +4212,8 @@
     <col min="3" max="3" width="10.7109375" style="4" customWidth="1"/>
     <col min="4" max="4" width="9.5703125" style="4" customWidth="1"/>
     <col min="5" max="7" width="12.7109375" style="1" customWidth="1"/>
-    <col min="8" max="11" width="25.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="28.7109375" style="1" customWidth="1"/>
+    <col min="9" max="11" width="25.7109375" style="1" customWidth="1"/>
     <col min="12" max="16384" width="16.140625" style="1"/>
   </cols>
   <sheetData>
@@ -4047,7 +4258,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="33.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>62</v>
       </c>
@@ -4060,11 +4271,14 @@
       <c r="D2" s="4">
         <v>0</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>63</v>
       </c>
@@ -4077,19 +4291,1747 @@
       <c r="D3" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="45" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="67.5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="90" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="4">
+        <v>2</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="67.5" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="4">
+        <v>1</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>103</v>
+      </c>
       <c r="L7" s="1" t="s">
         <v>15</v>
       </c>
     </row>
+    <row r="8" spans="1:13" ht="67.5" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0</v>
+      </c>
+      <c r="D9" s="4">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="J10" s="3"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
+      <c r="A10" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="4">
+        <v>1</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="56.25" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="4">
+        <v>2</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="56.25" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="4">
+        <v>2</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="56.25" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="4">
+        <v>2</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="4">
+        <v>0</v>
+      </c>
+      <c r="D14" s="4">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="4">
+        <v>0</v>
+      </c>
+      <c r="D15" s="4">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0</v>
+      </c>
+      <c r="D16" s="4">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>315</v>
+      </c>
       <c r="K16" s="4"/>
+    </row>
+    <row r="17" spans="1:10" ht="168.75" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="4">
+        <v>1</v>
+      </c>
+      <c r="D17" s="4">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="I17" s="4"/>
+      <c r="J17" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="4">
+        <v>0</v>
+      </c>
+      <c r="D18" s="4">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="4">
+        <v>1</v>
+      </c>
+      <c r="D19" s="4">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="4">
+        <v>1</v>
+      </c>
+      <c r="D20" s="4">
+        <v>0</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="4">
+        <v>1</v>
+      </c>
+      <c r="D21" s="4">
+        <v>0</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="4">
+        <v>0</v>
+      </c>
+      <c r="D22" s="4">
+        <v>1</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="4">
+        <v>0</v>
+      </c>
+      <c r="D23" s="4">
+        <v>1</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="4">
+        <v>0</v>
+      </c>
+      <c r="D24" s="4">
+        <v>1</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="4">
+        <v>0</v>
+      </c>
+      <c r="D25" s="4">
+        <v>1</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="4">
+        <v>0</v>
+      </c>
+      <c r="D26" s="4">
+        <v>1</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="4">
+        <v>0</v>
+      </c>
+      <c r="D27" s="4">
+        <v>1</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" s="4">
+        <v>0</v>
+      </c>
+      <c r="D28" s="4">
+        <v>1</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" s="4">
+        <v>0</v>
+      </c>
+      <c r="D29" s="4">
+        <v>1</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" s="4">
+        <v>0</v>
+      </c>
+      <c r="D30" s="4">
+        <v>1</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" s="4">
+        <v>0</v>
+      </c>
+      <c r="D31" s="4">
+        <v>1</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="4">
+        <v>0</v>
+      </c>
+      <c r="D32" s="4">
+        <v>1</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" s="4">
+        <v>0</v>
+      </c>
+      <c r="D33" s="4">
+        <v>1</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34" s="4">
+        <v>0</v>
+      </c>
+      <c r="D34" s="4">
+        <v>1</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" s="4">
+        <v>0</v>
+      </c>
+      <c r="D35" s="4">
+        <v>1</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36" s="4">
+        <v>0</v>
+      </c>
+      <c r="D36" s="4">
+        <v>1</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C37" s="4">
+        <v>0</v>
+      </c>
+      <c r="D37" s="4">
+        <v>1</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C38" s="4">
+        <v>0</v>
+      </c>
+      <c r="D38" s="4">
+        <v>1</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" s="4">
+        <v>0</v>
+      </c>
+      <c r="D39" s="4">
+        <v>1</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C40" s="4">
+        <v>0</v>
+      </c>
+      <c r="D40" s="4">
+        <v>1</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C41" s="4">
+        <v>1</v>
+      </c>
+      <c r="D41" s="4">
+        <v>0</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="67.5" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C42" s="4">
+        <v>1</v>
+      </c>
+      <c r="D42" s="4">
+        <v>0</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="101.25" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C43" s="4">
+        <v>1</v>
+      </c>
+      <c r="D43" s="4">
+        <v>0</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="90" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C44" s="4">
+        <v>1</v>
+      </c>
+      <c r="D44" s="4">
+        <v>0</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="56.25" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C45" s="4">
+        <v>1</v>
+      </c>
+      <c r="D45" s="4">
+        <v>0</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="67.5" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C46" s="4">
+        <v>1</v>
+      </c>
+      <c r="D46" s="4">
+        <v>0</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="123.75" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C47" s="4">
+        <v>1</v>
+      </c>
+      <c r="D47" s="4">
+        <v>0</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="101.25" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C48" s="4">
+        <v>1</v>
+      </c>
+      <c r="D48" s="4">
+        <v>0</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="101.25" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C49" s="4">
+        <v>1</v>
+      </c>
+      <c r="D49" s="4">
+        <v>0</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="101.25" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C50" s="4">
+        <v>1</v>
+      </c>
+      <c r="D50" s="4">
+        <v>0</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="78.75" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C51" s="4">
+        <v>1</v>
+      </c>
+      <c r="D51" s="4">
+        <v>0</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="J51" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="90" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C52" s="4">
+        <v>1</v>
+      </c>
+      <c r="D52" s="4">
+        <v>0</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="J52" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="123.75" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C53" s="4">
+        <v>1</v>
+      </c>
+      <c r="D53" s="4">
+        <v>0</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="J53" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="56.25" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C54" s="4">
+        <v>1</v>
+      </c>
+      <c r="D54" s="4">
+        <v>0</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="J54" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" ht="123.75" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C55" s="4">
+        <v>1</v>
+      </c>
+      <c r="D55" s="4">
+        <v>0</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="J55" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="78.75" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C56" s="4">
+        <v>1</v>
+      </c>
+      <c r="D56" s="4">
+        <v>0</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="90" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C57" s="4">
+        <v>1</v>
+      </c>
+      <c r="D57" s="4">
+        <v>0</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" ht="123.75" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C58" s="4">
+        <v>1</v>
+      </c>
+      <c r="D58" s="4">
+        <v>0</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="J58" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C59" s="4">
+        <v>1</v>
+      </c>
+      <c r="D59" s="4">
+        <v>0</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="J59" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C60" s="4">
+        <v>1</v>
+      </c>
+      <c r="D60" s="4">
+        <v>0</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" ht="56.25" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C61" s="4">
+        <v>1</v>
+      </c>
+      <c r="D61" s="4">
+        <v>0</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" ht="67.5" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C62" s="4">
+        <v>1</v>
+      </c>
+      <c r="D62" s="4">
+        <v>0</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="J62" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" ht="90" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C63" s="4">
+        <v>1</v>
+      </c>
+      <c r="D63" s="4">
+        <v>0</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="J63" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" ht="112.5" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C64" s="4">
+        <v>1</v>
+      </c>
+      <c r="D64" s="4">
+        <v>0</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="J64" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" ht="101.25" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C65" s="4">
+        <v>1</v>
+      </c>
+      <c r="D65" s="4">
+        <v>0</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="J65" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="112.5" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C66" s="4">
+        <v>1</v>
+      </c>
+      <c r="D66" s="4">
+        <v>0</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="J66" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" ht="78.75" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C67" s="4">
+        <v>1</v>
+      </c>
+      <c r="D67" s="4">
+        <v>0</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="J67" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" ht="90" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C68" s="4">
+        <v>1</v>
+      </c>
+      <c r="D68" s="4">
+        <v>0</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="J68" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" ht="157.5" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C69" s="4">
+        <v>1</v>
+      </c>
+      <c r="D69" s="4">
+        <v>0</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="J69" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" ht="135" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C70" s="4">
+        <v>1</v>
+      </c>
+      <c r="D70" s="4">
+        <v>0</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="J70" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C71" s="4">
+        <v>0</v>
+      </c>
+      <c r="D71" s="4">
+        <v>1</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="I71" s="1" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C72" s="4">
+        <v>0</v>
+      </c>
+      <c r="D72" s="4">
+        <v>1</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="I72" s="1" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C73" s="4">
+        <v>0</v>
+      </c>
+      <c r="D73" s="4">
+        <v>1</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="I73" s="1" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C74" s="4">
+        <v>0</v>
+      </c>
+      <c r="D74" s="4">
+        <v>1</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="I74" s="1" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C75" s="4">
+        <v>1</v>
+      </c>
+      <c r="D75" s="4">
+        <v>0</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="H75" s="1" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" ht="56.25" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C76" s="4">
+        <v>1</v>
+      </c>
+      <c r="D76" s="4">
+        <v>0</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="H76" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C77" s="4">
+        <v>0</v>
+      </c>
+      <c r="D77" s="4">
+        <v>1</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="I77" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" ht="112.5" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C78" s="4">
+        <v>1</v>
+      </c>
+      <c r="D78" s="4">
+        <v>0</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="H78" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="J78" s="1" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C79" s="4">
+        <v>0</v>
+      </c>
+      <c r="D79" s="4">
+        <v>1</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="I79" s="1" t="s">
+        <v>358</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Session Save & Load Functions
</commit_message>
<xml_diff>
--- a/intent-definition.xlsx
+++ b/intent-definition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\User\Documents\Code\Thesis\Symptom-Checker-Chatbot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FBC58B7-468A-4C4F-9CAE-2C3833EB513F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E49697-5DEF-4F8D-A729-0A1E05520DA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="321">
   <si>
     <t>parameters</t>
   </si>
@@ -975,6 +975,18 @@
   </si>
   <si>
     <t>{@sys.temperature:{Ano ang iyong temperatura?}{Ano ang temperatura ng iyong katawan?}}</t>
+  </si>
+  <si>
+    <t>{@sys.duration:{Again, how long?}{How long?}</t>
+  </si>
+  <si>
+    <t>{@duration_generic:{Again, how long?}{How long?}</t>
+  </si>
+  <si>
+    <t>{@sys.duration:{Muli, gaano katagal?}{Gaano katagal?}</t>
+  </si>
+  <si>
+    <t>{@duration_generic:{Muli, gaano katagal?}{Gaano katagal?}</t>
   </si>
 </sst>
 </file>
@@ -2184,8 +2196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{563BB99E-AECF-4E9F-90DC-16BA1EB2C1A9}">
   <dimension ref="A1:M81"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K75" sqref="K75"/>
+    <sheetView topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13:K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -2530,6 +2542,9 @@
       <c r="J13" s="1" t="s">
         <v>111</v>
       </c>
+      <c r="K13" s="1" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="14" spans="1:13" ht="67.5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
@@ -2555,6 +2570,9 @@
       </c>
       <c r="J14" s="1" t="s">
         <v>112</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
@@ -4071,8 +4089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AF69D1E-B293-4AC9-BAA2-CC12BCEF0879}">
   <dimension ref="A1:M81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I73" sqref="I73"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -4412,6 +4430,9 @@
       <c r="J13" s="1" t="s">
         <v>111</v>
       </c>
+      <c r="K13" s="1" t="s">
+        <v>319</v>
+      </c>
     </row>
     <row r="14" spans="1:13" ht="90" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
@@ -4437,6 +4458,9 @@
       </c>
       <c r="J14" s="1" t="s">
         <v>112</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">

</xml_diff>